<commit_message>
update docs: juc & mysql
</commit_message>
<xml_diff>
--- a/career/计划&复盘.xlsx
+++ b/career/计划&复盘.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\inotebook\career\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4358FAA9-4783-4D8C-A692-77122B5A510E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44231B0-72D1-493B-886B-6ED4EE38A590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="216">
   <si>
     <t>JVM</t>
   </si>
@@ -2695,6 +2695,45 @@
   <si>
     <t>8:30~12:10
 13:10~23:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Redis, MySQL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clickhouse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8:30~12:00
+13:30~18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atguigu,csnote</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>druid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10:00~12:00
+14:30~23:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9:30~12:30
+13:30~23:20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atguigu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:30~24:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3053,7 +3092,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3370,6 +3409,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="58" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3385,46 +3439,46 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3444,12 +3498,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3734,7 +3782,7 @@
   <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3782,7 +3830,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="114" t="s">
         <v>184</v>
       </c>
       <c r="B2" s="77"/>
@@ -3799,8 +3847,8 @@
       <c r="I2" s="98"/>
     </row>
     <row r="3" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="110"/>
-      <c r="B3" s="112" t="s">
+      <c r="A3" s="115"/>
+      <c r="B3" s="117" t="s">
         <v>85</v>
       </c>
       <c r="C3" s="80">
@@ -3816,8 +3864,8 @@
       <c r="I3" s="99"/>
     </row>
     <row r="4" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="110"/>
-      <c r="B4" s="110"/>
+      <c r="A4" s="115"/>
+      <c r="B4" s="115"/>
       <c r="C4" s="72">
         <v>44383</v>
       </c>
@@ -3831,8 +3879,8 @@
       <c r="I4" s="100"/>
     </row>
     <row r="5" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="110"/>
-      <c r="B5" s="110"/>
+      <c r="A5" s="115"/>
+      <c r="B5" s="115"/>
       <c r="C5" s="72">
         <v>44384</v>
       </c>
@@ -3846,8 +3894,8 @@
       <c r="I5" s="100"/>
     </row>
     <row r="6" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="110"/>
-      <c r="B6" s="110"/>
+      <c r="A6" s="115"/>
+      <c r="B6" s="115"/>
       <c r="C6" s="72">
         <v>44385</v>
       </c>
@@ -3865,8 +3913,8 @@
       <c r="I6" s="100"/>
     </row>
     <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="110"/>
-      <c r="B7" s="110"/>
+      <c r="A7" s="115"/>
+      <c r="B7" s="115"/>
       <c r="C7" s="72">
         <v>44386</v>
       </c>
@@ -3882,9 +3930,9 @@
       <c r="I7" s="100"/>
     </row>
     <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="110"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="108">
+      <c r="A8" s="115"/>
+      <c r="B8" s="115"/>
+      <c r="C8" s="113">
         <v>44387</v>
       </c>
       <c r="D8" s="71" t="s">
@@ -3903,9 +3951,9 @@
       <c r="I8" s="100"/>
     </row>
     <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="110"/>
-      <c r="B9" s="110"/>
-      <c r="C9" s="108"/>
+      <c r="A9" s="115"/>
+      <c r="B9" s="115"/>
+      <c r="C9" s="113"/>
       <c r="D9" s="70" t="s">
         <v>12</v>
       </c>
@@ -3922,8 +3970,8 @@
       <c r="I9" s="100"/>
     </row>
     <row r="10" spans="1:18" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="110"/>
-      <c r="B10" s="111"/>
+      <c r="A10" s="115"/>
+      <c r="B10" s="116"/>
       <c r="C10" s="83">
         <v>44388</v>
       </c>
@@ -3943,8 +3991,8 @@
       <c r="I10" s="101"/>
     </row>
     <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="110"/>
-      <c r="B11" s="112" t="s">
+      <c r="A11" s="115"/>
+      <c r="B11" s="117" t="s">
         <v>86</v>
       </c>
       <c r="C11" s="80">
@@ -3974,8 +4022,8 @@
       <c r="R11" s="39"/>
     </row>
     <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="110"/>
-      <c r="B12" s="110"/>
+      <c r="A12" s="115"/>
+      <c r="B12" s="115"/>
       <c r="C12" s="72">
         <v>44390</v>
       </c>
@@ -4003,8 +4051,8 @@
       <c r="R12" s="39"/>
     </row>
     <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="110"/>
-      <c r="B13" s="110"/>
+      <c r="A13" s="115"/>
+      <c r="B13" s="115"/>
       <c r="C13" s="72">
         <v>44391</v>
       </c>
@@ -4032,8 +4080,8 @@
       <c r="R13" s="39"/>
     </row>
     <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="110"/>
-      <c r="B14" s="110"/>
+      <c r="A14" s="115"/>
+      <c r="B14" s="115"/>
       <c r="C14" s="72">
         <v>44392</v>
       </c>
@@ -4061,8 +4109,8 @@
       <c r="R14" s="39"/>
     </row>
     <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="110"/>
-      <c r="B15" s="110"/>
+      <c r="A15" s="115"/>
+      <c r="B15" s="115"/>
       <c r="C15" s="72">
         <v>44393</v>
       </c>
@@ -4081,8 +4129,8 @@
       <c r="R15" s="39"/>
     </row>
     <row r="16" spans="1:18" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="110"/>
-      <c r="B16" s="110"/>
+      <c r="A16" s="115"/>
+      <c r="B16" s="115"/>
       <c r="C16" s="72">
         <v>44394</v>
       </c>
@@ -4107,8 +4155,8 @@
       <c r="R16" s="39"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="110"/>
-      <c r="B17" s="111"/>
+      <c r="A17" s="115"/>
+      <c r="B17" s="116"/>
       <c r="C17" s="83">
         <v>44395</v>
       </c>
@@ -4133,8 +4181,8 @@
       <c r="R17" s="39"/>
     </row>
     <row r="18" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="110"/>
-      <c r="B18" s="112" t="s">
+      <c r="A18" s="115"/>
+      <c r="B18" s="117" t="s">
         <v>82</v>
       </c>
       <c r="C18" s="80">
@@ -4163,8 +4211,8 @@
       <c r="R18" s="39"/>
     </row>
     <row r="19" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="110"/>
-      <c r="B19" s="110"/>
+      <c r="A19" s="115"/>
+      <c r="B19" s="115"/>
       <c r="C19" s="72">
         <v>44397</v>
       </c>
@@ -4195,8 +4243,8 @@
       <c r="R19" s="39"/>
     </row>
     <row r="20" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="110"/>
-      <c r="B20" s="110"/>
+      <c r="A20" s="115"/>
+      <c r="B20" s="115"/>
       <c r="C20" s="72">
         <v>44398</v>
       </c>
@@ -4227,8 +4275,8 @@
       <c r="R20" s="39"/>
     </row>
     <row r="21" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="110"/>
-      <c r="B21" s="110"/>
+      <c r="A21" s="115"/>
+      <c r="B21" s="115"/>
       <c r="C21" s="72">
         <v>44399</v>
       </c>
@@ -4259,8 +4307,8 @@
       <c r="R21" s="39"/>
     </row>
     <row r="22" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="110"/>
-      <c r="B22" s="110"/>
+      <c r="A22" s="115"/>
+      <c r="B22" s="115"/>
       <c r="C22" s="72">
         <v>44400</v>
       </c>
@@ -4279,8 +4327,8 @@
       <c r="R22" s="39"/>
     </row>
     <row r="23" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="110"/>
-      <c r="B23" s="110"/>
+      <c r="A23" s="115"/>
+      <c r="B23" s="115"/>
       <c r="C23" s="72">
         <v>44401</v>
       </c>
@@ -4300,22 +4348,26 @@
       <c r="I23" s="102" t="s">
         <v>192</v>
       </c>
-      <c r="L23" s="40" t="s">
+      <c r="L23" s="106" t="s">
         <v>185</v>
       </c>
-      <c r="M23" s="40" t="s">
+      <c r="M23" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="N23" s="40" t="s">
+      <c r="N23" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="O23" s="39"/>
-      <c r="Q23" s="39"/>
+      <c r="O23" s="112" t="s">
+        <v>211</v>
+      </c>
+      <c r="P23" s="111" t="s">
+        <v>208</v>
+      </c>
       <c r="R23" s="39"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="110"/>
-      <c r="B24" s="111"/>
+      <c r="A24" s="115"/>
+      <c r="B24" s="116"/>
       <c r="C24" s="83">
         <v>44402</v>
       </c>
@@ -4343,8 +4395,8 @@
       <c r="R24" s="39"/>
     </row>
     <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="110"/>
-      <c r="B25" s="112" t="s">
+      <c r="A25" s="115"/>
+      <c r="B25" s="117" t="s">
         <v>83</v>
       </c>
       <c r="C25" s="80">
@@ -4367,7 +4419,7 @@
       <c r="L25" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="M25" s="40" t="s">
+      <c r="M25" s="41" t="s">
         <v>47</v>
       </c>
       <c r="N25" s="40"/>
@@ -4376,23 +4428,25 @@
       <c r="R25" s="39"/>
     </row>
     <row r="26" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="110"/>
-      <c r="B26" s="110"/>
+      <c r="A26" s="115"/>
+      <c r="B26" s="115"/>
       <c r="C26" s="72">
         <v>44404</v>
       </c>
-      <c r="D26" s="71"/>
+      <c r="D26" s="71" t="s">
+        <v>207</v>
+      </c>
       <c r="E26" s="93"/>
       <c r="F26" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="133" t="s">
+      <c r="G26" s="108" t="s">
         <v>206</v>
       </c>
       <c r="H26" s="69">
         <v>13</v>
       </c>
-      <c r="I26" s="134" t="s">
+      <c r="I26" s="109" t="s">
         <v>4</v>
       </c>
       <c r="L26" s="40" t="s">
@@ -4403,19 +4457,25 @@
       <c r="Q26" s="39"/>
       <c r="R26" s="39"/>
     </row>
-    <row r="27" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="110"/>
-      <c r="B27" s="110"/>
+    <row r="27" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="115"/>
+      <c r="B27" s="115"/>
       <c r="C27" s="72">
         <v>44405</v>
       </c>
-      <c r="D27" s="71"/>
+      <c r="D27" s="71" t="s">
+        <v>185</v>
+      </c>
       <c r="E27" s="93"/>
       <c r="F27" s="74" t="s">
         <v>175</v>
       </c>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
+      <c r="G27" s="108" t="s">
+        <v>209</v>
+      </c>
+      <c r="H27" s="69">
+        <v>8</v>
+      </c>
       <c r="I27" s="100"/>
       <c r="L27" s="40" t="s">
         <v>70</v>
@@ -4425,20 +4485,30 @@
       <c r="Q27" s="39"/>
       <c r="R27" s="39"/>
     </row>
-    <row r="28" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="110"/>
-      <c r="B28" s="110"/>
+    <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="115"/>
+      <c r="B28" s="115"/>
       <c r="C28" s="72">
         <v>44406</v>
       </c>
-      <c r="D28" s="71"/>
-      <c r="E28" s="93"/>
+      <c r="D28" s="71" t="s">
+        <v>185</v>
+      </c>
+      <c r="E28" s="93" t="s">
+        <v>210</v>
+      </c>
       <c r="F28" s="74" t="s">
         <v>186</v>
       </c>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="100"/>
+      <c r="G28" s="108" t="s">
+        <v>212</v>
+      </c>
+      <c r="H28" s="69">
+        <v>11</v>
+      </c>
+      <c r="I28" s="110" t="s">
+        <v>185</v>
+      </c>
       <c r="L28" s="40" t="s">
         <v>72</v>
       </c>
@@ -4447,19 +4517,27 @@
       <c r="Q28" s="39"/>
       <c r="R28" s="39"/>
     </row>
-    <row r="29" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="110"/>
-      <c r="B29" s="110"/>
+    <row r="29" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="115"/>
+      <c r="B29" s="115"/>
       <c r="C29" s="72">
         <v>44407</v>
       </c>
-      <c r="D29" s="71"/>
-      <c r="E29" s="93"/>
+      <c r="D29" s="71" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="93" t="s">
+        <v>214</v>
+      </c>
       <c r="F29" s="74" t="s">
         <v>188</v>
       </c>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
+      <c r="G29" s="108" t="s">
+        <v>213</v>
+      </c>
+      <c r="H29" s="69">
+        <v>13</v>
+      </c>
       <c r="I29" s="100"/>
       <c r="L29" s="40" t="s">
         <v>73</v>
@@ -4470,18 +4548,26 @@
       <c r="R29" s="39"/>
     </row>
     <row r="30" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="110"/>
-      <c r="B30" s="110"/>
+      <c r="A30" s="115"/>
+      <c r="B30" s="115"/>
       <c r="C30" s="72">
         <v>44408</v>
       </c>
-      <c r="D30" s="71"/>
-      <c r="E30" s="93"/>
+      <c r="D30" s="71" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="93" t="s">
+        <v>214</v>
+      </c>
       <c r="F30" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
+      <c r="G30" s="69" t="s">
+        <v>215</v>
+      </c>
+      <c r="H30" s="69">
+        <v>9</v>
+      </c>
       <c r="I30" s="100"/>
       <c r="L30" s="40" t="s">
         <v>71</v>
@@ -4492,8 +4578,8 @@
       <c r="R30" s="39"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="111"/>
-      <c r="B31" s="111"/>
+      <c r="A31" s="116"/>
+      <c r="B31" s="116"/>
       <c r="C31" s="83">
         <v>44409</v>
       </c>
@@ -4713,10 +4799,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="129" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="19">
@@ -4735,8 +4821,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="117"/>
-      <c r="B3" s="115"/>
+      <c r="A3" s="126"/>
+      <c r="B3" s="122"/>
       <c r="C3" s="24">
         <v>44241</v>
       </c>
@@ -4747,8 +4833,8 @@
       <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="117"/>
-      <c r="B4" s="122" t="s">
+      <c r="A4" s="126"/>
+      <c r="B4" s="120" t="s">
         <v>82</v>
       </c>
       <c r="C4" s="19">
@@ -4767,8 +4853,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="117"/>
-      <c r="B5" s="114"/>
+      <c r="A5" s="126"/>
+      <c r="B5" s="121"/>
       <c r="C5" s="4">
         <v>44243</v>
       </c>
@@ -4785,9 +4871,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="117"/>
-      <c r="B6" s="114"/>
-      <c r="C6" s="125">
+      <c r="A6" s="126"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="118">
         <v>44244</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -4803,9 +4889,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="117"/>
-      <c r="B7" s="114"/>
-      <c r="C7" s="126"/>
+      <c r="A7" s="126"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="119"/>
       <c r="D7" s="5" t="s">
         <v>53</v>
       </c>
@@ -4821,8 +4907,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="117"/>
-      <c r="B8" s="114"/>
+      <c r="A8" s="126"/>
+      <c r="B8" s="121"/>
       <c r="C8" s="4">
         <v>44245</v>
       </c>
@@ -4841,8 +4927,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="117"/>
-      <c r="B9" s="114"/>
+      <c r="A9" s="126"/>
+      <c r="B9" s="121"/>
       <c r="C9" s="4">
         <v>44246</v>
       </c>
@@ -4861,8 +4947,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="117"/>
-      <c r="B10" s="114"/>
+      <c r="A10" s="126"/>
+      <c r="B10" s="121"/>
       <c r="C10" s="4">
         <v>44247</v>
       </c>
@@ -4873,8 +4959,8 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="117"/>
-      <c r="B11" s="115"/>
+      <c r="A11" s="126"/>
+      <c r="B11" s="122"/>
       <c r="C11" s="24">
         <v>44248</v>
       </c>
@@ -4891,8 +4977,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="117"/>
-      <c r="B12" s="120" t="s">
+      <c r="A12" s="126"/>
+      <c r="B12" s="123" t="s">
         <v>83</v>
       </c>
       <c r="C12" s="13">
@@ -4907,9 +4993,9 @@
       <c r="H12" s="17"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="117"/>
-      <c r="B13" s="120"/>
-      <c r="C13" s="125">
+      <c r="A13" s="126"/>
+      <c r="B13" s="123"/>
+      <c r="C13" s="118">
         <v>44250</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -4923,9 +5009,9 @@
       <c r="H13" s="17"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="117"/>
-      <c r="B14" s="114"/>
-      <c r="C14" s="126"/>
+      <c r="A14" s="126"/>
+      <c r="B14" s="121"/>
+      <c r="C14" s="119"/>
       <c r="D14" s="5" t="s">
         <v>60</v>
       </c>
@@ -4937,8 +5023,8 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="117"/>
-      <c r="B15" s="114"/>
+      <c r="A15" s="126"/>
+      <c r="B15" s="121"/>
       <c r="C15" s="4">
         <v>44251</v>
       </c>
@@ -4947,8 +5033,8 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="117"/>
-      <c r="B16" s="114"/>
+      <c r="A16" s="126"/>
+      <c r="B16" s="121"/>
       <c r="C16" s="4">
         <v>44252</v>
       </c>
@@ -4959,8 +5045,8 @@
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="117"/>
-      <c r="B17" s="114"/>
+      <c r="A17" s="126"/>
+      <c r="B17" s="121"/>
       <c r="C17" s="4">
         <v>44253</v>
       </c>
@@ -4971,9 +5057,9 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="117"/>
-      <c r="B18" s="114"/>
-      <c r="C18" s="125">
+      <c r="A18" s="126"/>
+      <c r="B18" s="121"/>
+      <c r="C18" s="118">
         <v>44254</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -4985,9 +5071,9 @@
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="124"/>
-      <c r="B19" s="123"/>
-      <c r="C19" s="126"/>
+      <c r="A19" s="128"/>
+      <c r="B19" s="124"/>
+      <c r="C19" s="119"/>
       <c r="D19" s="33" t="s">
         <v>62</v>
       </c>
@@ -4997,8 +5083,8 @@
       <c r="H19" s="36"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="118"/>
-      <c r="B20" s="115"/>
+      <c r="A20" s="127"/>
+      <c r="B20" s="122"/>
       <c r="C20" s="24">
         <v>44255</v>
       </c>
@@ -5011,10 +5097,10 @@
       <c r="H20" s="28"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="116" t="s">
+      <c r="A21" s="125" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="122" t="s">
+      <c r="B21" s="120" t="s">
         <v>85</v>
       </c>
       <c r="C21" s="19">
@@ -5029,8 +5115,8 @@
       <c r="H21" s="23"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="117"/>
-      <c r="B22" s="114"/>
+      <c r="A22" s="126"/>
+      <c r="B22" s="121"/>
       <c r="C22" s="4">
         <v>44257</v>
       </c>
@@ -5043,9 +5129,9 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="117"/>
-      <c r="B23" s="114"/>
-      <c r="C23" s="125">
+      <c r="A23" s="126"/>
+      <c r="B23" s="121"/>
+      <c r="C23" s="118">
         <v>44258</v>
       </c>
       <c r="D23" s="5" t="s">
@@ -5057,9 +5143,9 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="117"/>
-      <c r="B24" s="114"/>
-      <c r="C24" s="126"/>
+      <c r="A24" s="126"/>
+      <c r="B24" s="121"/>
+      <c r="C24" s="119"/>
       <c r="D24" s="5" t="s">
         <v>66</v>
       </c>
@@ -5071,9 +5157,9 @@
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="117"/>
-      <c r="B25" s="114"/>
-      <c r="C25" s="125">
+      <c r="A25" s="126"/>
+      <c r="B25" s="121"/>
+      <c r="C25" s="118">
         <v>44259</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -5087,9 +5173,9 @@
       <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="117"/>
-      <c r="B26" s="114"/>
-      <c r="C26" s="126"/>
+      <c r="A26" s="126"/>
+      <c r="B26" s="121"/>
+      <c r="C26" s="119"/>
       <c r="D26" s="5" t="s">
         <v>69</v>
       </c>
@@ -5099,8 +5185,8 @@
       <c r="H26" s="8"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="117"/>
-      <c r="B27" s="114"/>
+      <c r="A27" s="126"/>
+      <c r="B27" s="121"/>
       <c r="C27" s="4">
         <v>44260</v>
       </c>
@@ -5111,8 +5197,8 @@
       <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="117"/>
-      <c r="B28" s="114"/>
+      <c r="A28" s="126"/>
+      <c r="B28" s="121"/>
       <c r="C28" s="4">
         <v>44261</v>
       </c>
@@ -5123,8 +5209,8 @@
       <c r="H28" s="8"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="117"/>
-      <c r="B29" s="115"/>
+      <c r="A29" s="126"/>
+      <c r="B29" s="122"/>
       <c r="C29" s="24">
         <v>44262</v>
       </c>
@@ -5135,8 +5221,8 @@
       <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="117"/>
-      <c r="B30" s="122" t="s">
+      <c r="A30" s="126"/>
+      <c r="B30" s="120" t="s">
         <v>86</v>
       </c>
       <c r="C30" s="19">
@@ -5149,8 +5235,8 @@
       <c r="H30" s="23"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="117"/>
-      <c r="B31" s="114"/>
+      <c r="A31" s="126"/>
+      <c r="B31" s="121"/>
       <c r="C31" s="4">
         <v>44264</v>
       </c>
@@ -5161,8 +5247,8 @@
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="117"/>
-      <c r="B32" s="114"/>
+      <c r="A32" s="126"/>
+      <c r="B32" s="121"/>
       <c r="C32" s="4">
         <v>44265</v>
       </c>
@@ -5173,8 +5259,8 @@
       <c r="H32" s="8"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="117"/>
-      <c r="B33" s="114"/>
+      <c r="A33" s="126"/>
+      <c r="B33" s="121"/>
       <c r="C33" s="4">
         <v>44266</v>
       </c>
@@ -5185,8 +5271,8 @@
       <c r="H33" s="8"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="117"/>
-      <c r="B34" s="114"/>
+      <c r="A34" s="126"/>
+      <c r="B34" s="121"/>
       <c r="C34" s="4">
         <v>44267</v>
       </c>
@@ -5197,8 +5283,8 @@
       <c r="H34" s="8"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="117"/>
-      <c r="B35" s="114"/>
+      <c r="A35" s="126"/>
+      <c r="B35" s="121"/>
       <c r="C35" s="4">
         <v>44268</v>
       </c>
@@ -5209,8 +5295,8 @@
       <c r="H35" s="8"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="117"/>
-      <c r="B36" s="115"/>
+      <c r="A36" s="126"/>
+      <c r="B36" s="122"/>
       <c r="C36" s="24">
         <v>44269</v>
       </c>
@@ -5221,8 +5307,8 @@
       <c r="H36" s="28"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="117"/>
-      <c r="B37" s="122" t="s">
+      <c r="A37" s="126"/>
+      <c r="B37" s="120" t="s">
         <v>82</v>
       </c>
       <c r="C37" s="19">
@@ -5237,8 +5323,8 @@
       <c r="H37" s="23"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="117"/>
-      <c r="B38" s="114"/>
+      <c r="A38" s="126"/>
+      <c r="B38" s="121"/>
       <c r="C38" s="4">
         <v>44271</v>
       </c>
@@ -5253,8 +5339,8 @@
       <c r="H38" s="8"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="117"/>
-      <c r="B39" s="114"/>
+      <c r="A39" s="126"/>
+      <c r="B39" s="121"/>
       <c r="C39" s="4">
         <v>44272</v>
       </c>
@@ -5269,8 +5355,8 @@
       <c r="H39" s="8"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="117"/>
-      <c r="B40" s="114"/>
+      <c r="A40" s="126"/>
+      <c r="B40" s="121"/>
       <c r="C40" s="4">
         <v>44273</v>
       </c>
@@ -5285,8 +5371,8 @@
       <c r="H40" s="8"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="117"/>
-      <c r="B41" s="114"/>
+      <c r="A41" s="126"/>
+      <c r="B41" s="121"/>
       <c r="C41" s="4">
         <v>44274</v>
       </c>
@@ -5301,8 +5387,8 @@
       <c r="H41" s="8"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="117"/>
-      <c r="B42" s="114"/>
+      <c r="A42" s="126"/>
+      <c r="B42" s="121"/>
       <c r="C42" s="4">
         <v>44275</v>
       </c>
@@ -5317,8 +5403,8 @@
       <c r="H42" s="8"/>
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="117"/>
-      <c r="B43" s="115"/>
+      <c r="A43" s="126"/>
+      <c r="B43" s="122"/>
       <c r="C43" s="24">
         <v>44276</v>
       </c>
@@ -5333,8 +5419,8 @@
       <c r="H43" s="28"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="117"/>
-      <c r="B44" s="120" t="s">
+      <c r="A44" s="126"/>
+      <c r="B44" s="123" t="s">
         <v>83</v>
       </c>
       <c r="C44" s="13">
@@ -5351,8 +5437,8 @@
       <c r="H44" s="17"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="117"/>
-      <c r="B45" s="114"/>
+      <c r="A45" s="126"/>
+      <c r="B45" s="121"/>
       <c r="C45" s="4">
         <v>44278</v>
       </c>
@@ -5367,8 +5453,8 @@
       <c r="H45" s="8"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="117"/>
-      <c r="B46" s="114"/>
+      <c r="A46" s="126"/>
+      <c r="B46" s="121"/>
       <c r="C46" s="4">
         <v>44279</v>
       </c>
@@ -5385,8 +5471,8 @@
       <c r="H46" s="8"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="117"/>
-      <c r="B47" s="114"/>
+      <c r="A47" s="126"/>
+      <c r="B47" s="121"/>
       <c r="C47" s="4">
         <v>44280</v>
       </c>
@@ -5403,8 +5489,8 @@
       <c r="H47" s="8"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="117"/>
-      <c r="B48" s="114"/>
+      <c r="A48" s="126"/>
+      <c r="B48" s="121"/>
       <c r="C48" s="4">
         <v>44281</v>
       </c>
@@ -5419,8 +5505,8 @@
       <c r="H48" s="8"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="117"/>
-      <c r="B49" s="114"/>
+      <c r="A49" s="126"/>
+      <c r="B49" s="121"/>
       <c r="C49" s="4">
         <v>44282</v>
       </c>
@@ -5437,8 +5523,8 @@
       <c r="H49" s="8"/>
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="118"/>
-      <c r="B50" s="115"/>
+      <c r="A50" s="127"/>
+      <c r="B50" s="122"/>
       <c r="C50" s="24">
         <v>44283</v>
       </c>
@@ -5453,10 +5539,10 @@
       <c r="H50" s="28"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="116" t="s">
+      <c r="A51" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="121" t="s">
+      <c r="B51" s="129" t="s">
         <v>88</v>
       </c>
       <c r="C51" s="19">
@@ -5475,8 +5561,8 @@
       <c r="H51" s="23"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="117"/>
-      <c r="B52" s="114"/>
+      <c r="A52" s="126"/>
+      <c r="B52" s="121"/>
       <c r="C52" s="4">
         <v>44285</v>
       </c>
@@ -5491,9 +5577,9 @@
       <c r="H52" s="8"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="117"/>
-      <c r="B53" s="114"/>
-      <c r="C53" s="119">
+      <c r="A53" s="126"/>
+      <c r="B53" s="121"/>
+      <c r="C53" s="131">
         <v>44286</v>
       </c>
       <c r="D53" s="5" t="s">
@@ -5507,9 +5593,9 @@
       <c r="H53" s="8"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="117"/>
-      <c r="B54" s="114"/>
-      <c r="C54" s="119"/>
+      <c r="A54" s="126"/>
+      <c r="B54" s="121"/>
+      <c r="C54" s="131"/>
       <c r="D54" s="5" t="s">
         <v>70</v>
       </c>
@@ -5521,8 +5607,8 @@
       <c r="H54" s="8"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="117"/>
-      <c r="B55" s="114"/>
+      <c r="A55" s="126"/>
+      <c r="B55" s="121"/>
       <c r="C55" s="4">
         <v>44287</v>
       </c>
@@ -5533,8 +5619,8 @@
       <c r="H55" s="8"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="117"/>
-      <c r="B56" s="114"/>
+      <c r="A56" s="126"/>
+      <c r="B56" s="121"/>
       <c r="C56" s="4">
         <v>44288</v>
       </c>
@@ -5547,8 +5633,8 @@
       <c r="H56" s="8"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="117"/>
-      <c r="B57" s="114"/>
+      <c r="A57" s="126"/>
+      <c r="B57" s="121"/>
       <c r="C57" s="4">
         <v>44289</v>
       </c>
@@ -5561,8 +5647,8 @@
       <c r="H57" s="8"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="117"/>
-      <c r="B58" s="115"/>
+      <c r="A58" s="126"/>
+      <c r="B58" s="122"/>
       <c r="C58" s="24">
         <v>44290</v>
       </c>
@@ -5575,8 +5661,8 @@
       <c r="H58" s="28"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="117"/>
-      <c r="B59" s="121" t="s">
+      <c r="A59" s="126"/>
+      <c r="B59" s="129" t="s">
         <v>86</v>
       </c>
       <c r="C59" s="19">
@@ -5591,8 +5677,8 @@
       <c r="H59" s="23"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="117"/>
-      <c r="B60" s="114"/>
+      <c r="A60" s="126"/>
+      <c r="B60" s="121"/>
       <c r="C60" s="4">
         <v>44292</v>
       </c>
@@ -5607,8 +5693,8 @@
       <c r="H60" s="8"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="117"/>
-      <c r="B61" s="114"/>
+      <c r="A61" s="126"/>
+      <c r="B61" s="121"/>
       <c r="C61" s="4">
         <v>44293</v>
       </c>
@@ -5623,8 +5709,8 @@
       <c r="H61" s="8"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="117"/>
-      <c r="B62" s="114"/>
+      <c r="A62" s="126"/>
+      <c r="B62" s="121"/>
       <c r="C62" s="4">
         <v>44294</v>
       </c>
@@ -5639,8 +5725,8 @@
       <c r="H62" s="8"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="117"/>
-      <c r="B63" s="114"/>
+      <c r="A63" s="126"/>
+      <c r="B63" s="121"/>
       <c r="C63" s="4">
         <v>44295</v>
       </c>
@@ -5651,8 +5737,8 @@
       <c r="H63" s="8"/>
     </row>
     <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="117"/>
-      <c r="B64" s="114"/>
+      <c r="A64" s="126"/>
+      <c r="B64" s="121"/>
       <c r="C64" s="4">
         <v>44296</v>
       </c>
@@ -5663,8 +5749,8 @@
       <c r="H64" s="8"/>
     </row>
     <row r="65" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="117"/>
-      <c r="B65" s="115"/>
+      <c r="A65" s="126"/>
+      <c r="B65" s="122"/>
       <c r="C65" s="24">
         <v>44297</v>
       </c>
@@ -5679,8 +5765,8 @@
       <c r="H65" s="28"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="117"/>
-      <c r="B66" s="113" t="s">
+      <c r="A66" s="126"/>
+      <c r="B66" s="130" t="s">
         <v>82</v>
       </c>
       <c r="C66" s="13">
@@ -5697,8 +5783,8 @@
       <c r="H66" s="17"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="117"/>
-      <c r="B67" s="114"/>
+      <c r="A67" s="126"/>
+      <c r="B67" s="121"/>
       <c r="C67" s="4">
         <v>44299</v>
       </c>
@@ -5713,8 +5799,8 @@
       <c r="H67" s="8"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="117"/>
-      <c r="B68" s="114"/>
+      <c r="A68" s="126"/>
+      <c r="B68" s="121"/>
       <c r="C68" s="4">
         <v>44300</v>
       </c>
@@ -5727,8 +5813,8 @@
       <c r="H68" s="8"/>
     </row>
     <row r="69" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="118"/>
-      <c r="B69" s="115"/>
+      <c r="A69" s="127"/>
+      <c r="B69" s="122"/>
       <c r="C69" s="24">
         <v>44301</v>
       </c>
@@ -5740,11 +5826,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="A51:A69"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="B51:B58"/>
+    <mergeCell ref="B59:B65"/>
     <mergeCell ref="B30:B36"/>
     <mergeCell ref="B21:B29"/>
     <mergeCell ref="B12:B20"/>
@@ -5753,12 +5840,11 @@
     <mergeCell ref="A2:A20"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B37:B43"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="A51:A69"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="B51:B58"/>
-    <mergeCell ref="B59:B65"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5815,10 +5901,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="121" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="121" t="s">
         <v>146</v>
       </c>
       <c r="C2" s="42">
@@ -5837,8 +5923,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="114"/>
-      <c r="B3" s="115"/>
+      <c r="A3" s="121"/>
+      <c r="B3" s="122"/>
       <c r="C3" s="54">
         <v>44094</v>
       </c>
@@ -5855,8 +5941,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="114"/>
-      <c r="B4" s="120" t="s">
+      <c r="A4" s="121"/>
+      <c r="B4" s="123" t="s">
         <v>123</v>
       </c>
       <c r="C4" s="51">
@@ -5875,8 +5961,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="114"/>
-      <c r="B5" s="114"/>
+      <c r="A5" s="121"/>
+      <c r="B5" s="121"/>
       <c r="C5" s="42">
         <v>44096</v>
       </c>
@@ -5893,8 +5979,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="114"/>
-      <c r="B6" s="114"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="121"/>
       <c r="C6" s="42">
         <v>44097</v>
       </c>
@@ -5911,8 +5997,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="114"/>
-      <c r="B7" s="114"/>
+      <c r="A7" s="121"/>
+      <c r="B7" s="121"/>
       <c r="C7" s="42">
         <v>44098</v>
       </c>
@@ -5929,8 +6015,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="114"/>
-      <c r="B8" s="114"/>
+      <c r="A8" s="121"/>
+      <c r="B8" s="121"/>
       <c r="C8" s="42">
         <v>44099</v>
       </c>
@@ -5947,8 +6033,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="114"/>
-      <c r="B9" s="114"/>
+      <c r="A9" s="121"/>
+      <c r="B9" s="121"/>
       <c r="C9" s="42">
         <v>44100</v>
       </c>
@@ -5965,8 +6051,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="115"/>
-      <c r="B10" s="115"/>
+      <c r="A10" s="122"/>
+      <c r="B10" s="122"/>
       <c r="C10" s="54">
         <v>44101</v>
       </c>
@@ -5983,10 +6069,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="129" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="120" t="s">
         <v>88</v>
       </c>
       <c r="C11" s="59">
@@ -6005,8 +6091,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="114"/>
-      <c r="B12" s="114"/>
+      <c r="A12" s="121"/>
+      <c r="B12" s="121"/>
       <c r="C12" s="42">
         <v>44103</v>
       </c>
@@ -6017,8 +6103,8 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="114"/>
-      <c r="B13" s="114"/>
+      <c r="A13" s="121"/>
+      <c r="B13" s="121"/>
       <c r="C13" s="42">
         <v>44104</v>
       </c>
@@ -6029,8 +6115,8 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="114"/>
-      <c r="B14" s="114"/>
+      <c r="A14" s="121"/>
+      <c r="B14" s="121"/>
       <c r="C14" s="42">
         <v>44105</v>
       </c>
@@ -6045,8 +6131,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="114"/>
-      <c r="B15" s="114"/>
+      <c r="A15" s="121"/>
+      <c r="B15" s="121"/>
       <c r="C15" s="42">
         <v>44106</v>
       </c>
@@ -6063,8 +6149,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="114"/>
-      <c r="B16" s="114"/>
+      <c r="A16" s="121"/>
+      <c r="B16" s="121"/>
       <c r="C16" s="42">
         <v>44107</v>
       </c>
@@ -6081,8 +6167,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="114"/>
-      <c r="B17" s="115"/>
+      <c r="A17" s="121"/>
+      <c r="B17" s="122"/>
       <c r="C17" s="54">
         <v>44108</v>
       </c>
@@ -6099,11 +6185,11 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="114"/>
-      <c r="B18" s="122" t="s">
+      <c r="A18" s="121"/>
+      <c r="B18" s="120" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="127">
+      <c r="C18" s="132">
         <v>44109</v>
       </c>
       <c r="D18" s="60" t="s">
@@ -6119,9 +6205,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="114"/>
-      <c r="B19" s="132"/>
-      <c r="C19" s="128"/>
+      <c r="A19" s="121"/>
+      <c r="B19" s="137"/>
+      <c r="C19" s="133"/>
       <c r="D19" s="43" t="s">
         <v>129</v>
       </c>
@@ -6135,9 +6221,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="114"/>
-      <c r="B20" s="132"/>
-      <c r="C20" s="128"/>
+      <c r="A20" s="121"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="133"/>
       <c r="D20" s="43" t="s">
         <v>101</v>
       </c>
@@ -6151,8 +6237,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="114"/>
-      <c r="B21" s="114"/>
+      <c r="A21" s="121"/>
+      <c r="B21" s="121"/>
       <c r="C21" s="42">
         <v>44110</v>
       </c>
@@ -6163,8 +6249,8 @@
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="114"/>
-      <c r="B22" s="114"/>
+      <c r="A22" s="121"/>
+      <c r="B22" s="121"/>
       <c r="C22" s="42">
         <v>44111</v>
       </c>
@@ -6175,8 +6261,8 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="114"/>
-      <c r="B23" s="114"/>
+      <c r="A23" s="121"/>
+      <c r="B23" s="121"/>
       <c r="C23" s="42">
         <v>44112</v>
       </c>
@@ -6187,8 +6273,8 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="114"/>
-      <c r="B24" s="114"/>
+      <c r="A24" s="121"/>
+      <c r="B24" s="121"/>
       <c r="C24" s="42">
         <v>44113</v>
       </c>
@@ -6199,9 +6285,9 @@
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="114"/>
-      <c r="B25" s="114"/>
-      <c r="C25" s="128">
+      <c r="A25" s="121"/>
+      <c r="B25" s="121"/>
+      <c r="C25" s="133">
         <v>44114</v>
       </c>
       <c r="D25" s="43" t="s">
@@ -6217,9 +6303,9 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="114"/>
-      <c r="B26" s="114"/>
-      <c r="C26" s="128"/>
+      <c r="A26" s="121"/>
+      <c r="B26" s="121"/>
+      <c r="C26" s="133"/>
       <c r="D26" s="43" t="s">
         <v>102</v>
       </c>
@@ -6233,8 +6319,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="114"/>
-      <c r="B27" s="115"/>
+      <c r="A27" s="121"/>
+      <c r="B27" s="122"/>
       <c r="C27" s="54">
         <v>44115</v>
       </c>
@@ -6251,8 +6337,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="114"/>
-      <c r="B28" s="122" t="s">
+      <c r="A28" s="121"/>
+      <c r="B28" s="120" t="s">
         <v>82</v>
       </c>
       <c r="C28" s="59">
@@ -6265,8 +6351,8 @@
       <c r="H28" s="23"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="114"/>
-      <c r="B29" s="114"/>
+      <c r="A29" s="121"/>
+      <c r="B29" s="121"/>
       <c r="C29" s="42">
         <v>44117</v>
       </c>
@@ -6283,8 +6369,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="114"/>
-      <c r="B30" s="114"/>
+      <c r="A30" s="121"/>
+      <c r="B30" s="121"/>
       <c r="C30" s="42">
         <v>44118</v>
       </c>
@@ -6295,8 +6381,8 @@
       <c r="H30" s="8"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="114"/>
-      <c r="B31" s="114"/>
+      <c r="A31" s="121"/>
+      <c r="B31" s="121"/>
       <c r="C31" s="42">
         <v>44119</v>
       </c>
@@ -6313,8 +6399,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="114"/>
-      <c r="B32" s="114"/>
+      <c r="A32" s="121"/>
+      <c r="B32" s="121"/>
       <c r="C32" s="42">
         <v>44120</v>
       </c>
@@ -6325,8 +6411,8 @@
       <c r="H32" s="8"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="114"/>
-      <c r="B33" s="114"/>
+      <c r="A33" s="121"/>
+      <c r="B33" s="121"/>
       <c r="C33" s="42">
         <v>44121</v>
       </c>
@@ -6343,9 +6429,9 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="114"/>
-      <c r="B34" s="114"/>
-      <c r="C34" s="128">
+      <c r="A34" s="121"/>
+      <c r="B34" s="121"/>
+      <c r="C34" s="133">
         <v>44122</v>
       </c>
       <c r="D34" s="43" t="s">
@@ -6361,9 +6447,9 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="114"/>
-      <c r="B35" s="115"/>
-      <c r="C35" s="129"/>
+      <c r="A35" s="121"/>
+      <c r="B35" s="122"/>
+      <c r="C35" s="134"/>
       <c r="D35" s="55" t="s">
         <v>103</v>
       </c>
@@ -6377,8 +6463,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="114"/>
-      <c r="B36" s="122" t="s">
+      <c r="A36" s="121"/>
+      <c r="B36" s="120" t="s">
         <v>83</v>
       </c>
       <c r="C36" s="59">
@@ -6391,8 +6477,8 @@
       <c r="H36" s="23"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="114"/>
-      <c r="B37" s="114"/>
+      <c r="A37" s="121"/>
+      <c r="B37" s="121"/>
       <c r="C37" s="42">
         <v>44124</v>
       </c>
@@ -6403,8 +6489,8 @@
       <c r="H37" s="8"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="114"/>
-      <c r="B38" s="114"/>
+      <c r="A38" s="121"/>
+      <c r="B38" s="121"/>
       <c r="C38" s="42">
         <v>44125</v>
       </c>
@@ -6415,8 +6501,8 @@
       <c r="H38" s="8"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="114"/>
-      <c r="B39" s="114"/>
+      <c r="A39" s="121"/>
+      <c r="B39" s="121"/>
       <c r="C39" s="42">
         <v>44126</v>
       </c>
@@ -6427,8 +6513,8 @@
       <c r="H39" s="8"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="114"/>
-      <c r="B40" s="114"/>
+      <c r="A40" s="121"/>
+      <c r="B40" s="121"/>
       <c r="C40" s="42">
         <v>44127</v>
       </c>
@@ -6439,8 +6525,8 @@
       <c r="H40" s="8"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="114"/>
-      <c r="B41" s="114"/>
+      <c r="A41" s="121"/>
+      <c r="B41" s="121"/>
       <c r="C41" s="42">
         <v>44128</v>
       </c>
@@ -6457,8 +6543,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="114"/>
-      <c r="B42" s="115"/>
+      <c r="A42" s="121"/>
+      <c r="B42" s="122"/>
       <c r="C42" s="54">
         <v>44129</v>
       </c>
@@ -6469,8 +6555,8 @@
       <c r="H42" s="28"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="114"/>
-      <c r="B43" s="113" t="s">
+      <c r="A43" s="121"/>
+      <c r="B43" s="130" t="s">
         <v>138</v>
       </c>
       <c r="C43" s="51">
@@ -6489,8 +6575,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="114"/>
-      <c r="B44" s="114"/>
+      <c r="A44" s="121"/>
+      <c r="B44" s="121"/>
       <c r="C44" s="42">
         <v>44131</v>
       </c>
@@ -6507,8 +6593,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="114"/>
-      <c r="B45" s="114"/>
+      <c r="A45" s="121"/>
+      <c r="B45" s="121"/>
       <c r="C45" s="42">
         <v>44132</v>
       </c>
@@ -6525,8 +6611,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="114"/>
-      <c r="B46" s="114"/>
+      <c r="A46" s="121"/>
+      <c r="B46" s="121"/>
       <c r="C46" s="42">
         <v>44133</v>
       </c>
@@ -6537,8 +6623,8 @@
       <c r="H46" s="8"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="114"/>
-      <c r="B47" s="114"/>
+      <c r="A47" s="121"/>
+      <c r="B47" s="121"/>
       <c r="C47" s="42">
         <v>44134</v>
       </c>
@@ -6549,8 +6635,8 @@
       <c r="H47" s="8"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="114"/>
-      <c r="B48" s="114"/>
+      <c r="A48" s="121"/>
+      <c r="B48" s="121"/>
       <c r="C48" s="42">
         <v>44135</v>
       </c>
@@ -6561,8 +6647,8 @@
       <c r="H48" s="8"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="115"/>
-      <c r="B49" s="115"/>
+      <c r="A49" s="122"/>
+      <c r="B49" s="122"/>
       <c r="C49" s="54">
         <v>44136</v>
       </c>
@@ -6579,10 +6665,10 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="121" t="s">
+      <c r="A50" s="129" t="s">
         <v>140</v>
       </c>
-      <c r="B50" s="122" t="s">
+      <c r="B50" s="120" t="s">
         <v>88</v>
       </c>
       <c r="C50" s="59">
@@ -6595,8 +6681,8 @@
       <c r="H50" s="23"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="114"/>
-      <c r="B51" s="114"/>
+      <c r="A51" s="121"/>
+      <c r="B51" s="121"/>
       <c r="C51" s="42">
         <v>44138</v>
       </c>
@@ -6613,8 +6699,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="114"/>
-      <c r="B52" s="114"/>
+      <c r="A52" s="121"/>
+      <c r="B52" s="121"/>
       <c r="C52" s="42">
         <v>44139</v>
       </c>
@@ -6625,8 +6711,8 @@
       <c r="H52" s="8"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="114"/>
-      <c r="B53" s="114"/>
+      <c r="A53" s="121"/>
+      <c r="B53" s="121"/>
       <c r="C53" s="42">
         <v>44140</v>
       </c>
@@ -6643,8 +6729,8 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="114"/>
-      <c r="B54" s="114"/>
+      <c r="A54" s="121"/>
+      <c r="B54" s="121"/>
       <c r="C54" s="42">
         <v>44141</v>
       </c>
@@ -6655,8 +6741,8 @@
       <c r="H54" s="8"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="114"/>
-      <c r="B55" s="114"/>
+      <c r="A55" s="121"/>
+      <c r="B55" s="121"/>
       <c r="C55" s="42">
         <v>44142</v>
       </c>
@@ -6667,8 +6753,8 @@
       <c r="H55" s="8"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="114"/>
-      <c r="B56" s="115"/>
+      <c r="A56" s="121"/>
+      <c r="B56" s="122"/>
       <c r="C56" s="54">
         <v>44143</v>
       </c>
@@ -6685,8 +6771,8 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="114"/>
-      <c r="B57" s="122" t="s">
+      <c r="A57" s="121"/>
+      <c r="B57" s="120" t="s">
         <v>86</v>
       </c>
       <c r="C57" s="59">
@@ -6705,8 +6791,8 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="114"/>
-      <c r="B58" s="114"/>
+      <c r="A58" s="121"/>
+      <c r="B58" s="121"/>
       <c r="C58" s="42">
         <v>44145</v>
       </c>
@@ -6723,8 +6809,8 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="114"/>
-      <c r="B59" s="114"/>
+      <c r="A59" s="121"/>
+      <c r="B59" s="121"/>
       <c r="C59" s="42">
         <v>44146</v>
       </c>
@@ -6741,8 +6827,8 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="114"/>
-      <c r="B60" s="114"/>
+      <c r="A60" s="121"/>
+      <c r="B60" s="121"/>
       <c r="C60" s="42">
         <v>44147</v>
       </c>
@@ -6759,8 +6845,8 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="114"/>
-      <c r="B61" s="114"/>
+      <c r="A61" s="121"/>
+      <c r="B61" s="121"/>
       <c r="C61" s="42">
         <v>44148</v>
       </c>
@@ -6771,8 +6857,8 @@
       <c r="H61" s="8"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="114"/>
-      <c r="B62" s="114"/>
+      <c r="A62" s="121"/>
+      <c r="B62" s="121"/>
       <c r="C62" s="42">
         <v>44149</v>
       </c>
@@ -6789,8 +6875,8 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="114"/>
-      <c r="B63" s="115"/>
+      <c r="A63" s="121"/>
+      <c r="B63" s="122"/>
       <c r="C63" s="54">
         <v>44150</v>
       </c>
@@ -6807,8 +6893,8 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="114"/>
-      <c r="B64" s="122" t="s">
+      <c r="A64" s="121"/>
+      <c r="B64" s="120" t="s">
         <v>82</v>
       </c>
       <c r="C64" s="59">
@@ -6827,8 +6913,8 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="114"/>
-      <c r="B65" s="114"/>
+      <c r="A65" s="121"/>
+      <c r="B65" s="121"/>
       <c r="C65" s="42">
         <v>44152</v>
       </c>
@@ -6845,8 +6931,8 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="114"/>
-      <c r="B66" s="114"/>
+      <c r="A66" s="121"/>
+      <c r="B66" s="121"/>
       <c r="C66" s="42">
         <v>44153</v>
       </c>
@@ -6857,9 +6943,9 @@
       <c r="H66" s="8"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="114"/>
-      <c r="B67" s="114"/>
-      <c r="C67" s="130">
+      <c r="A67" s="121"/>
+      <c r="B67" s="121"/>
+      <c r="C67" s="135">
         <v>44154</v>
       </c>
       <c r="D67" s="43" t="s">
@@ -6875,9 +6961,9 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="114"/>
-      <c r="B68" s="114"/>
-      <c r="C68" s="131"/>
+      <c r="A68" s="121"/>
+      <c r="B68" s="121"/>
+      <c r="C68" s="136"/>
       <c r="D68" s="43" t="s">
         <v>107</v>
       </c>
@@ -6891,8 +6977,8 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="114"/>
-      <c r="B69" s="114"/>
+      <c r="A69" s="121"/>
+      <c r="B69" s="121"/>
       <c r="C69" s="42">
         <v>44155</v>
       </c>
@@ -6903,8 +6989,8 @@
       <c r="H69" s="8"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="114"/>
-      <c r="B70" s="114"/>
+      <c r="A70" s="121"/>
+      <c r="B70" s="121"/>
       <c r="C70" s="42">
         <v>44156</v>
       </c>
@@ -6915,8 +7001,8 @@
       <c r="H70" s="8"/>
     </row>
     <row r="71" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="114"/>
-      <c r="B71" s="115"/>
+      <c r="A71" s="121"/>
+      <c r="B71" s="122"/>
       <c r="C71" s="54">
         <v>44157</v>
       </c>
@@ -6933,8 +7019,8 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="114"/>
-      <c r="B72" s="113" t="s">
+      <c r="A72" s="121"/>
+      <c r="B72" s="130" t="s">
         <v>123</v>
       </c>
       <c r="C72" s="51">
@@ -6953,8 +7039,8 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="114"/>
-      <c r="B73" s="114"/>
+      <c r="A73" s="121"/>
+      <c r="B73" s="121"/>
       <c r="C73" s="42">
         <v>44159</v>
       </c>
@@ -6965,8 +7051,8 @@
       <c r="H73" s="8"/>
     </row>
     <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="115"/>
-      <c r="B74" s="115"/>
+      <c r="A74" s="122"/>
+      <c r="B74" s="122"/>
       <c r="C74" s="54">
         <v>44160</v>
       </c>
@@ -6984,6 +7070,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A11:A49"/>
+    <mergeCell ref="A50:A74"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="B11:B17"/>
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="C25:C26"/>
@@ -6995,13 +7088,6 @@
     <mergeCell ref="B18:B27"/>
     <mergeCell ref="B28:B35"/>
     <mergeCell ref="B36:B42"/>
-    <mergeCell ref="A11:A49"/>
-    <mergeCell ref="A50:A74"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="B11:B17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add gather for docs
</commit_message>
<xml_diff>
--- a/career/计划&复盘.xlsx
+++ b/career/计划&复盘.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\inotebook\career\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8DA9C9-0A70-403C-A5F4-D4A4360A1DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB09F97-B342-492A-9C32-7B95642CDC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16875" yWindow="2430" windowWidth="16065" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20535" yWindow="3045" windowWidth="16065" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="7月计划" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="236">
   <si>
     <t>JVM</t>
   </si>
@@ -2932,6 +2932,10 @@
   <si>
     <t>18:30~20:30
 22:30~23:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZK, Kafka</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3079,7 +3083,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3137,6 +3141,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3334,7 +3344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3702,13 +3712,19 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="58" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3717,52 +3733,46 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3782,6 +3792,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4067,7 +4080,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4117,7 +4130,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="129" t="s">
         <v>219</v>
       </c>
       <c r="B2" s="73"/>
@@ -4134,8 +4147,8 @@
       <c r="I2" s="92"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="127"/>
-      <c r="B3" s="129" t="s">
+      <c r="A3" s="126"/>
+      <c r="B3" s="131" t="s">
         <v>85</v>
       </c>
       <c r="C3" s="76">
@@ -4151,8 +4164,8 @@
       <c r="I3" s="93"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="127"/>
-      <c r="B4" s="127"/>
+      <c r="A4" s="126"/>
+      <c r="B4" s="126"/>
       <c r="C4" s="102">
         <v>44383</v>
       </c>
@@ -4166,8 +4179,8 @@
       <c r="I4" s="94"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="127"/>
-      <c r="B5" s="127"/>
+      <c r="A5" s="126"/>
+      <c r="B5" s="126"/>
       <c r="C5" s="102">
         <v>44384</v>
       </c>
@@ -4181,8 +4194,8 @@
       <c r="I5" s="94"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="127"/>
-      <c r="B6" s="127"/>
+      <c r="A6" s="126"/>
+      <c r="B6" s="126"/>
       <c r="C6" s="102">
         <v>44385</v>
       </c>
@@ -4200,8 +4213,8 @@
       <c r="I6" s="94"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="127"/>
-      <c r="B7" s="127"/>
+      <c r="A7" s="126"/>
+      <c r="B7" s="126"/>
       <c r="C7" s="102">
         <v>44386</v>
       </c>
@@ -4217,9 +4230,9 @@
       <c r="I7" s="94"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="127"/>
-      <c r="B8" s="127"/>
-      <c r="C8" s="125">
+      <c r="A8" s="126"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="128">
         <v>44387</v>
       </c>
       <c r="D8" s="68" t="s">
@@ -4238,9 +4251,9 @@
       <c r="I8" s="94"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="127"/>
-      <c r="B9" s="127"/>
-      <c r="C9" s="125"/>
+      <c r="A9" s="126"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="128"/>
       <c r="D9" s="67" t="s">
         <v>12</v>
       </c>
@@ -4257,8 +4270,8 @@
       <c r="I9" s="94"/>
     </row>
     <row r="10" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="127"/>
-      <c r="B10" s="128"/>
+      <c r="A10" s="126"/>
+      <c r="B10" s="130"/>
       <c r="C10" s="79">
         <v>44388</v>
       </c>
@@ -4278,8 +4291,8 @@
       <c r="I10" s="95"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="127"/>
-      <c r="B11" s="129" t="s">
+      <c r="A11" s="126"/>
+      <c r="B11" s="131" t="s">
         <v>86</v>
       </c>
       <c r="C11" s="76">
@@ -4304,8 +4317,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="127"/>
-      <c r="B12" s="127"/>
+      <c r="A12" s="126"/>
+      <c r="B12" s="126"/>
       <c r="C12" s="102">
         <v>44390</v>
       </c>
@@ -4328,8 +4341,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="127"/>
-      <c r="B13" s="127"/>
+      <c r="A13" s="126"/>
+      <c r="B13" s="126"/>
       <c r="C13" s="102">
         <v>44391</v>
       </c>
@@ -4352,8 +4365,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="127"/>
-      <c r="B14" s="127"/>
+      <c r="A14" s="126"/>
+      <c r="B14" s="126"/>
       <c r="C14" s="102">
         <v>44392</v>
       </c>
@@ -4376,8 +4389,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="127"/>
-      <c r="B15" s="127"/>
+      <c r="A15" s="126"/>
+      <c r="B15" s="126"/>
       <c r="C15" s="102">
         <v>44393</v>
       </c>
@@ -4392,8 +4405,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="127"/>
-      <c r="B16" s="127"/>
+      <c r="A16" s="126"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="102">
         <v>44394</v>
       </c>
@@ -4413,8 +4426,8 @@
       <c r="I16" s="94"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="127"/>
-      <c r="B17" s="128"/>
+      <c r="A17" s="126"/>
+      <c r="B17" s="130"/>
       <c r="C17" s="79">
         <v>44395</v>
       </c>
@@ -4434,8 +4447,8 @@
       <c r="I17" s="95"/>
     </row>
     <row r="18" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="127"/>
-      <c r="B18" s="129" t="s">
+      <c r="A18" s="126"/>
+      <c r="B18" s="131" t="s">
         <v>82</v>
       </c>
       <c r="C18" s="76">
@@ -4460,8 +4473,8 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="127"/>
-      <c r="B19" s="127"/>
+      <c r="A19" s="126"/>
+      <c r="B19" s="126"/>
       <c r="C19" s="102">
         <v>44397</v>
       </c>
@@ -4488,8 +4501,8 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="127"/>
-      <c r="B20" s="127"/>
+      <c r="A20" s="126"/>
+      <c r="B20" s="126"/>
       <c r="C20" s="102">
         <v>44398</v>
       </c>
@@ -4516,8 +4529,8 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="127"/>
-      <c r="B21" s="127"/>
+      <c r="A21" s="126"/>
+      <c r="B21" s="126"/>
       <c r="C21" s="102">
         <v>44399</v>
       </c>
@@ -4544,8 +4557,8 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="127"/>
-      <c r="B22" s="127"/>
+      <c r="A22" s="126"/>
+      <c r="B22" s="126"/>
       <c r="C22" s="102">
         <v>44400</v>
       </c>
@@ -4560,8 +4573,8 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="127"/>
-      <c r="B23" s="127"/>
+      <c r="A23" s="126"/>
+      <c r="B23" s="126"/>
       <c r="C23" s="102">
         <v>44401</v>
       </c>
@@ -4598,8 +4611,8 @@
       </c>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="127"/>
-      <c r="B24" s="128"/>
+      <c r="A24" s="126"/>
+      <c r="B24" s="130"/>
       <c r="C24" s="79">
         <v>44402</v>
       </c>
@@ -4624,8 +4637,8 @@
       <c r="N24" s="38"/>
     </row>
     <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="127"/>
-      <c r="B25" s="129" t="s">
+      <c r="A25" s="126"/>
+      <c r="B25" s="131" t="s">
         <v>83</v>
       </c>
       <c r="C25" s="76">
@@ -4654,8 +4667,8 @@
       <c r="N25" s="38"/>
     </row>
     <row r="26" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="127"/>
-      <c r="B26" s="127"/>
+      <c r="A26" s="126"/>
+      <c r="B26" s="126"/>
       <c r="C26" s="102">
         <v>44404</v>
       </c>
@@ -4680,8 +4693,8 @@
       </c>
     </row>
     <row r="27" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="127"/>
-      <c r="B27" s="127"/>
+      <c r="A27" s="126"/>
+      <c r="B27" s="126"/>
       <c r="C27" s="102">
         <v>44405</v>
       </c>
@@ -4704,8 +4717,8 @@
       </c>
     </row>
     <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="127"/>
-      <c r="B28" s="127"/>
+      <c r="A28" s="126"/>
+      <c r="B28" s="126"/>
       <c r="C28" s="102">
         <v>44406</v>
       </c>
@@ -4732,8 +4745,8 @@
       </c>
     </row>
     <row r="29" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="127"/>
-      <c r="B29" s="127"/>
+      <c r="A29" s="126"/>
+      <c r="B29" s="126"/>
       <c r="C29" s="102">
         <v>44407</v>
       </c>
@@ -4758,8 +4771,8 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="127"/>
-      <c r="B30" s="127"/>
+      <c r="A30" s="126"/>
+      <c r="B30" s="126"/>
       <c r="C30" s="102">
         <v>44408</v>
       </c>
@@ -4784,8 +4797,8 @@
       </c>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="128"/>
-      <c r="B31" s="128"/>
+      <c r="A31" s="130"/>
+      <c r="B31" s="130"/>
       <c r="C31" s="79">
         <v>44409</v>
       </c>
@@ -4812,10 +4825,10 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="131" t="s">
+      <c r="A32" s="127" t="s">
         <v>220</v>
       </c>
-      <c r="B32" s="130" t="s">
+      <c r="B32" s="125" t="s">
         <v>85</v>
       </c>
       <c r="C32" s="108">
@@ -4846,8 +4859,8 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="131"/>
-      <c r="B33" s="127"/>
+      <c r="A33" s="127"/>
+      <c r="B33" s="126"/>
       <c r="C33" s="107">
         <v>44411</v>
       </c>
@@ -4873,8 +4886,8 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="131"/>
-      <c r="B34" s="127"/>
+      <c r="A34" s="127"/>
+      <c r="B34" s="126"/>
       <c r="C34" s="107">
         <v>44412</v>
       </c>
@@ -4902,8 +4915,8 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="131"/>
-      <c r="B35" s="127"/>
+      <c r="A35" s="127"/>
+      <c r="B35" s="126"/>
       <c r="C35" s="107">
         <v>44413</v>
       </c>
@@ -4927,8 +4940,8 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="131"/>
-      <c r="B36" s="127"/>
+      <c r="A36" s="127"/>
+      <c r="B36" s="126"/>
       <c r="C36" s="107">
         <v>44414</v>
       </c>
@@ -4946,8 +4959,8 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="131"/>
-      <c r="B37" s="127"/>
+      <c r="A37" s="127"/>
+      <c r="B37" s="126"/>
       <c r="C37" s="107">
         <v>44415</v>
       </c>
@@ -4971,12 +4984,12 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="131"/>
-      <c r="B38" s="127"/>
+      <c r="A38" s="127"/>
+      <c r="B38" s="126"/>
       <c r="C38" s="107">
         <v>44416</v>
       </c>
-      <c r="D38" s="103" t="s">
+      <c r="D38" s="152" t="s">
         <v>229</v>
       </c>
       <c r="E38" s="117" t="s">
@@ -4996,8 +5009,8 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="131"/>
-      <c r="B39" s="127" t="s">
+      <c r="A39" s="127"/>
+      <c r="B39" s="126" t="s">
         <v>222</v>
       </c>
       <c r="C39" s="107">
@@ -5023,8 +5036,8 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="131"/>
-      <c r="B40" s="127"/>
+      <c r="A40" s="127"/>
+      <c r="B40" s="126"/>
       <c r="C40" s="107">
         <v>44418</v>
       </c>
@@ -5048,12 +5061,12 @@
       </c>
     </row>
     <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="131"/>
-      <c r="B41" s="127"/>
+      <c r="A41" s="127"/>
+      <c r="B41" s="126"/>
       <c r="C41" s="107">
         <v>44419</v>
       </c>
-      <c r="D41" s="103" t="s">
+      <c r="D41" s="152" t="s">
         <v>175</v>
       </c>
       <c r="E41" s="117"/>
@@ -5072,26 +5085,32 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="131"/>
-      <c r="B42" s="127"/>
+      <c r="A42" s="127"/>
+      <c r="B42" s="126"/>
       <c r="C42" s="107">
         <v>44420</v>
       </c>
-      <c r="D42" s="103"/>
+      <c r="D42" s="103" t="s">
+        <v>235</v>
+      </c>
       <c r="E42" s="117"/>
       <c r="F42" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="G42" s="103"/>
-      <c r="H42" s="103"/>
+      <c r="G42" s="103" t="s">
+        <v>232</v>
+      </c>
+      <c r="H42" s="103">
+        <v>3</v>
+      </c>
       <c r="I42" s="94"/>
       <c r="L42" s="38" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="131"/>
-      <c r="B43" s="127"/>
+      <c r="A43" s="127"/>
+      <c r="B43" s="126"/>
       <c r="C43" s="107">
         <v>44421</v>
       </c>
@@ -5108,8 +5127,8 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="131"/>
-      <c r="B44" s="127"/>
+      <c r="A44" s="127"/>
+      <c r="B44" s="126"/>
       <c r="C44" s="107">
         <v>44422</v>
       </c>
@@ -5126,8 +5145,8 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="131"/>
-      <c r="B45" s="127"/>
+      <c r="A45" s="127"/>
+      <c r="B45" s="126"/>
       <c r="C45" s="107">
         <v>44423</v>
       </c>
@@ -5144,8 +5163,8 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="131"/>
-      <c r="B46" s="127" t="s">
+      <c r="A46" s="127"/>
+      <c r="B46" s="126" t="s">
         <v>223</v>
       </c>
       <c r="C46" s="107">
@@ -5159,8 +5178,8 @@
       <c r="I46" s="94"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="131"/>
-      <c r="B47" s="127"/>
+      <c r="A47" s="127"/>
+      <c r="B47" s="126"/>
       <c r="C47" s="107">
         <v>44425</v>
       </c>
@@ -5172,8 +5191,8 @@
       <c r="I47" s="94"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="131"/>
-      <c r="B48" s="127"/>
+      <c r="A48" s="127"/>
+      <c r="B48" s="126"/>
       <c r="C48" s="107">
         <v>44426</v>
       </c>
@@ -5185,8 +5204,8 @@
       <c r="I48" s="94"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="131"/>
-      <c r="B49" s="127"/>
+      <c r="A49" s="127"/>
+      <c r="B49" s="126"/>
       <c r="C49" s="107">
         <v>44427</v>
       </c>
@@ -5198,8 +5217,8 @@
       <c r="I49" s="94"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="131"/>
-      <c r="B50" s="127"/>
+      <c r="A50" s="127"/>
+      <c r="B50" s="126"/>
       <c r="C50" s="107">
         <v>44428</v>
       </c>
@@ -5211,8 +5230,8 @@
       <c r="I50" s="94"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="131"/>
-      <c r="B51" s="127"/>
+      <c r="A51" s="127"/>
+      <c r="B51" s="126"/>
       <c r="C51" s="107">
         <v>44429</v>
       </c>
@@ -5224,8 +5243,8 @@
       <c r="I51" s="94"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="131"/>
-      <c r="B52" s="127"/>
+      <c r="A52" s="127"/>
+      <c r="B52" s="126"/>
       <c r="C52" s="107">
         <v>44430</v>
       </c>
@@ -5237,8 +5256,8 @@
       <c r="I52" s="94"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="131"/>
-      <c r="B53" s="127" t="s">
+      <c r="A53" s="127"/>
+      <c r="B53" s="126" t="s">
         <v>123</v>
       </c>
       <c r="C53" s="107">
@@ -5252,8 +5271,8 @@
       <c r="I53" s="94"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="131"/>
-      <c r="B54" s="127"/>
+      <c r="A54" s="127"/>
+      <c r="B54" s="126"/>
       <c r="C54" s="107">
         <v>44432</v>
       </c>
@@ -5265,8 +5284,8 @@
       <c r="I54" s="94"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="131"/>
-      <c r="B55" s="127"/>
+      <c r="A55" s="127"/>
+      <c r="B55" s="126"/>
       <c r="C55" s="107">
         <v>44433</v>
       </c>
@@ -5278,8 +5297,8 @@
       <c r="I55" s="94"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="131"/>
-      <c r="B56" s="127"/>
+      <c r="A56" s="127"/>
+      <c r="B56" s="126"/>
       <c r="C56" s="107">
         <v>44434</v>
       </c>
@@ -5291,8 +5310,8 @@
       <c r="I56" s="94"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="131"/>
-      <c r="B57" s="127"/>
+      <c r="A57" s="127"/>
+      <c r="B57" s="126"/>
       <c r="C57" s="107">
         <v>44435</v>
       </c>
@@ -5304,8 +5323,8 @@
       <c r="I57" s="94"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="131"/>
-      <c r="B58" s="127"/>
+      <c r="A58" s="127"/>
+      <c r="B58" s="126"/>
       <c r="C58" s="107">
         <v>44436</v>
       </c>
@@ -5317,8 +5336,8 @@
       <c r="I58" s="94"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="130"/>
-      <c r="B59" s="127"/>
+      <c r="A59" s="125"/>
+      <c r="B59" s="126"/>
       <c r="C59" s="107">
         <v>44437</v>
       </c>
@@ -5331,17 +5350,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="B39:B45"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="B53:B59"/>
-    <mergeCell ref="A32:A59"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="A2:A31"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B17"/>
     <mergeCell ref="B18:B24"/>
     <mergeCell ref="B25:B31"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="B53:B59"/>
+    <mergeCell ref="A32:A59"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5399,10 +5418,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="139" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="140" t="s">
+      <c r="B2" s="143" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="17">
@@ -5421,8 +5440,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="136"/>
-      <c r="B3" s="134"/>
+      <c r="A3" s="140"/>
+      <c r="B3" s="136"/>
       <c r="C3" s="22">
         <v>44241</v>
       </c>
@@ -5433,8 +5452,8 @@
       <c r="H3" s="26"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="136"/>
-      <c r="B4" s="141" t="s">
+      <c r="A4" s="140"/>
+      <c r="B4" s="134" t="s">
         <v>82</v>
       </c>
       <c r="C4" s="17">
@@ -5453,8 +5472,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="136"/>
-      <c r="B5" s="133"/>
+      <c r="A5" s="140"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="2">
         <v>44243</v>
       </c>
@@ -5471,9 +5490,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="136"/>
-      <c r="B6" s="133"/>
-      <c r="C6" s="144">
+      <c r="A6" s="140"/>
+      <c r="B6" s="135"/>
+      <c r="C6" s="132">
         <v>44244</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -5489,9 +5508,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="136"/>
-      <c r="B7" s="133"/>
-      <c r="C7" s="145"/>
+      <c r="A7" s="140"/>
+      <c r="B7" s="135"/>
+      <c r="C7" s="133"/>
       <c r="D7" s="3" t="s">
         <v>53</v>
       </c>
@@ -5507,8 +5526,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="136"/>
-      <c r="B8" s="133"/>
+      <c r="A8" s="140"/>
+      <c r="B8" s="135"/>
       <c r="C8" s="2">
         <v>44245</v>
       </c>
@@ -5527,8 +5546,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="136"/>
-      <c r="B9" s="133"/>
+      <c r="A9" s="140"/>
+      <c r="B9" s="135"/>
       <c r="C9" s="2">
         <v>44246</v>
       </c>
@@ -5547,8 +5566,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="136"/>
-      <c r="B10" s="133"/>
+      <c r="A10" s="140"/>
+      <c r="B10" s="135"/>
       <c r="C10" s="2">
         <v>44247</v>
       </c>
@@ -5559,8 +5578,8 @@
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="136"/>
-      <c r="B11" s="134"/>
+      <c r="A11" s="140"/>
+      <c r="B11" s="136"/>
       <c r="C11" s="22">
         <v>44248</v>
       </c>
@@ -5577,8 +5596,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="136"/>
-      <c r="B12" s="139" t="s">
+      <c r="A12" s="140"/>
+      <c r="B12" s="137" t="s">
         <v>83</v>
       </c>
       <c r="C12" s="11">
@@ -5593,9 +5612,9 @@
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="136"/>
-      <c r="B13" s="139"/>
-      <c r="C13" s="144">
+      <c r="A13" s="140"/>
+      <c r="B13" s="137"/>
+      <c r="C13" s="132">
         <v>44250</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -5609,9 +5628,9 @@
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="136"/>
-      <c r="B14" s="133"/>
-      <c r="C14" s="145"/>
+      <c r="A14" s="140"/>
+      <c r="B14" s="135"/>
+      <c r="C14" s="133"/>
       <c r="D14" s="3" t="s">
         <v>60</v>
       </c>
@@ -5623,8 +5642,8 @@
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="136"/>
-      <c r="B15" s="133"/>
+      <c r="A15" s="140"/>
+      <c r="B15" s="135"/>
       <c r="C15" s="2">
         <v>44251</v>
       </c>
@@ -5633,8 +5652,8 @@
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="136"/>
-      <c r="B16" s="133"/>
+      <c r="A16" s="140"/>
+      <c r="B16" s="135"/>
       <c r="C16" s="2">
         <v>44252</v>
       </c>
@@ -5645,8 +5664,8 @@
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="136"/>
-      <c r="B17" s="133"/>
+      <c r="A17" s="140"/>
+      <c r="B17" s="135"/>
       <c r="C17" s="2">
         <v>44253</v>
       </c>
@@ -5657,9 +5676,9 @@
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="136"/>
-      <c r="B18" s="133"/>
-      <c r="C18" s="144">
+      <c r="A18" s="140"/>
+      <c r="B18" s="135"/>
+      <c r="C18" s="132">
         <v>44254</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -5671,9 +5690,9 @@
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="143"/>
-      <c r="B19" s="142"/>
-      <c r="C19" s="145"/>
+      <c r="A19" s="142"/>
+      <c r="B19" s="138"/>
+      <c r="C19" s="133"/>
       <c r="D19" s="31" t="s">
         <v>62</v>
       </c>
@@ -5683,8 +5702,8 @@
       <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="137"/>
-      <c r="B20" s="134"/>
+      <c r="A20" s="141"/>
+      <c r="B20" s="136"/>
       <c r="C20" s="22">
         <v>44255</v>
       </c>
@@ -5697,10 +5716,10 @@
       <c r="H20" s="26"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="135" t="s">
+      <c r="A21" s="139" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="141" t="s">
+      <c r="B21" s="134" t="s">
         <v>85</v>
       </c>
       <c r="C21" s="17">
@@ -5715,8 +5734,8 @@
       <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="136"/>
-      <c r="B22" s="133"/>
+      <c r="A22" s="140"/>
+      <c r="B22" s="135"/>
       <c r="C22" s="2">
         <v>44257</v>
       </c>
@@ -5729,9 +5748,9 @@
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="136"/>
-      <c r="B23" s="133"/>
-      <c r="C23" s="144">
+      <c r="A23" s="140"/>
+      <c r="B23" s="135"/>
+      <c r="C23" s="132">
         <v>44258</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -5743,9 +5762,9 @@
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="136"/>
-      <c r="B24" s="133"/>
-      <c r="C24" s="145"/>
+      <c r="A24" s="140"/>
+      <c r="B24" s="135"/>
+      <c r="C24" s="133"/>
       <c r="D24" s="3" t="s">
         <v>66</v>
       </c>
@@ -5757,9 +5776,9 @@
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="136"/>
-      <c r="B25" s="133"/>
-      <c r="C25" s="144">
+      <c r="A25" s="140"/>
+      <c r="B25" s="135"/>
+      <c r="C25" s="132">
         <v>44259</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -5773,9 +5792,9 @@
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="136"/>
-      <c r="B26" s="133"/>
-      <c r="C26" s="145"/>
+      <c r="A26" s="140"/>
+      <c r="B26" s="135"/>
+      <c r="C26" s="133"/>
       <c r="D26" s="3" t="s">
         <v>69</v>
       </c>
@@ -5785,8 +5804,8 @@
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="136"/>
-      <c r="B27" s="133"/>
+      <c r="A27" s="140"/>
+      <c r="B27" s="135"/>
       <c r="C27" s="2">
         <v>44260</v>
       </c>
@@ -5797,8 +5816,8 @@
       <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="136"/>
-      <c r="B28" s="133"/>
+      <c r="A28" s="140"/>
+      <c r="B28" s="135"/>
       <c r="C28" s="2">
         <v>44261</v>
       </c>
@@ -5809,8 +5828,8 @@
       <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="136"/>
-      <c r="B29" s="134"/>
+      <c r="A29" s="140"/>
+      <c r="B29" s="136"/>
       <c r="C29" s="22">
         <v>44262</v>
       </c>
@@ -5821,8 +5840,8 @@
       <c r="H29" s="26"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="136"/>
-      <c r="B30" s="141" t="s">
+      <c r="A30" s="140"/>
+      <c r="B30" s="134" t="s">
         <v>86</v>
       </c>
       <c r="C30" s="17">
@@ -5835,8 +5854,8 @@
       <c r="H30" s="21"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="136"/>
-      <c r="B31" s="133"/>
+      <c r="A31" s="140"/>
+      <c r="B31" s="135"/>
       <c r="C31" s="2">
         <v>44264</v>
       </c>
@@ -5847,8 +5866,8 @@
       <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="136"/>
-      <c r="B32" s="133"/>
+      <c r="A32" s="140"/>
+      <c r="B32" s="135"/>
       <c r="C32" s="2">
         <v>44265</v>
       </c>
@@ -5859,8 +5878,8 @@
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="136"/>
-      <c r="B33" s="133"/>
+      <c r="A33" s="140"/>
+      <c r="B33" s="135"/>
       <c r="C33" s="2">
         <v>44266</v>
       </c>
@@ -5871,8 +5890,8 @@
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="136"/>
-      <c r="B34" s="133"/>
+      <c r="A34" s="140"/>
+      <c r="B34" s="135"/>
       <c r="C34" s="2">
         <v>44267</v>
       </c>
@@ -5883,8 +5902,8 @@
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="136"/>
-      <c r="B35" s="133"/>
+      <c r="A35" s="140"/>
+      <c r="B35" s="135"/>
       <c r="C35" s="2">
         <v>44268</v>
       </c>
@@ -5895,8 +5914,8 @@
       <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="136"/>
-      <c r="B36" s="134"/>
+      <c r="A36" s="140"/>
+      <c r="B36" s="136"/>
       <c r="C36" s="22">
         <v>44269</v>
       </c>
@@ -5907,8 +5926,8 @@
       <c r="H36" s="26"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="136"/>
-      <c r="B37" s="141" t="s">
+      <c r="A37" s="140"/>
+      <c r="B37" s="134" t="s">
         <v>82</v>
       </c>
       <c r="C37" s="17">
@@ -5923,8 +5942,8 @@
       <c r="H37" s="21"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="136"/>
-      <c r="B38" s="133"/>
+      <c r="A38" s="140"/>
+      <c r="B38" s="135"/>
       <c r="C38" s="2">
         <v>44271</v>
       </c>
@@ -5939,8 +5958,8 @@
       <c r="H38" s="6"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="136"/>
-      <c r="B39" s="133"/>
+      <c r="A39" s="140"/>
+      <c r="B39" s="135"/>
       <c r="C39" s="2">
         <v>44272</v>
       </c>
@@ -5955,8 +5974,8 @@
       <c r="H39" s="6"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="136"/>
-      <c r="B40" s="133"/>
+      <c r="A40" s="140"/>
+      <c r="B40" s="135"/>
       <c r="C40" s="2">
         <v>44273</v>
       </c>
@@ -5971,8 +5990,8 @@
       <c r="H40" s="6"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="136"/>
-      <c r="B41" s="133"/>
+      <c r="A41" s="140"/>
+      <c r="B41" s="135"/>
       <c r="C41" s="2">
         <v>44274</v>
       </c>
@@ -5987,8 +6006,8 @@
       <c r="H41" s="6"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="136"/>
-      <c r="B42" s="133"/>
+      <c r="A42" s="140"/>
+      <c r="B42" s="135"/>
       <c r="C42" s="2">
         <v>44275</v>
       </c>
@@ -6003,8 +6022,8 @@
       <c r="H42" s="6"/>
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="136"/>
-      <c r="B43" s="134"/>
+      <c r="A43" s="140"/>
+      <c r="B43" s="136"/>
       <c r="C43" s="22">
         <v>44276</v>
       </c>
@@ -6019,8 +6038,8 @@
       <c r="H43" s="26"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="136"/>
-      <c r="B44" s="139" t="s">
+      <c r="A44" s="140"/>
+      <c r="B44" s="137" t="s">
         <v>83</v>
       </c>
       <c r="C44" s="11">
@@ -6037,8 +6056,8 @@
       <c r="H44" s="15"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="136"/>
-      <c r="B45" s="133"/>
+      <c r="A45" s="140"/>
+      <c r="B45" s="135"/>
       <c r="C45" s="2">
         <v>44278</v>
       </c>
@@ -6053,8 +6072,8 @@
       <c r="H45" s="6"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="136"/>
-      <c r="B46" s="133"/>
+      <c r="A46" s="140"/>
+      <c r="B46" s="135"/>
       <c r="C46" s="2">
         <v>44279</v>
       </c>
@@ -6071,8 +6090,8 @@
       <c r="H46" s="6"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="136"/>
-      <c r="B47" s="133"/>
+      <c r="A47" s="140"/>
+      <c r="B47" s="135"/>
       <c r="C47" s="2">
         <v>44280</v>
       </c>
@@ -6089,8 +6108,8 @@
       <c r="H47" s="6"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="136"/>
-      <c r="B48" s="133"/>
+      <c r="A48" s="140"/>
+      <c r="B48" s="135"/>
       <c r="C48" s="2">
         <v>44281</v>
       </c>
@@ -6105,8 +6124,8 @@
       <c r="H48" s="6"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="136"/>
-      <c r="B49" s="133"/>
+      <c r="A49" s="140"/>
+      <c r="B49" s="135"/>
       <c r="C49" s="2">
         <v>44282</v>
       </c>
@@ -6123,8 +6142,8 @@
       <c r="H49" s="6"/>
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="137"/>
-      <c r="B50" s="134"/>
+      <c r="A50" s="141"/>
+      <c r="B50" s="136"/>
       <c r="C50" s="22">
         <v>44283</v>
       </c>
@@ -6139,10 +6158,10 @@
       <c r="H50" s="26"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="135" t="s">
+      <c r="A51" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="140" t="s">
+      <c r="B51" s="143" t="s">
         <v>88</v>
       </c>
       <c r="C51" s="17">
@@ -6161,8 +6180,8 @@
       <c r="H51" s="21"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="136"/>
-      <c r="B52" s="133"/>
+      <c r="A52" s="140"/>
+      <c r="B52" s="135"/>
       <c r="C52" s="2">
         <v>44285</v>
       </c>
@@ -6177,9 +6196,9 @@
       <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="136"/>
-      <c r="B53" s="133"/>
-      <c r="C53" s="138">
+      <c r="A53" s="140"/>
+      <c r="B53" s="135"/>
+      <c r="C53" s="145">
         <v>44286</v>
       </c>
       <c r="D53" s="3" t="s">
@@ -6193,9 +6212,9 @@
       <c r="H53" s="6"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="136"/>
-      <c r="B54" s="133"/>
-      <c r="C54" s="138"/>
+      <c r="A54" s="140"/>
+      <c r="B54" s="135"/>
+      <c r="C54" s="145"/>
       <c r="D54" s="3" t="s">
         <v>70</v>
       </c>
@@ -6207,8 +6226,8 @@
       <c r="H54" s="6"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="136"/>
-      <c r="B55" s="133"/>
+      <c r="A55" s="140"/>
+      <c r="B55" s="135"/>
       <c r="C55" s="2">
         <v>44287</v>
       </c>
@@ -6219,8 +6238,8 @@
       <c r="H55" s="6"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="136"/>
-      <c r="B56" s="133"/>
+      <c r="A56" s="140"/>
+      <c r="B56" s="135"/>
       <c r="C56" s="2">
         <v>44288</v>
       </c>
@@ -6233,8 +6252,8 @@
       <c r="H56" s="6"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="136"/>
-      <c r="B57" s="133"/>
+      <c r="A57" s="140"/>
+      <c r="B57" s="135"/>
       <c r="C57" s="2">
         <v>44289</v>
       </c>
@@ -6247,8 +6266,8 @@
       <c r="H57" s="6"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="136"/>
-      <c r="B58" s="134"/>
+      <c r="A58" s="140"/>
+      <c r="B58" s="136"/>
       <c r="C58" s="22">
         <v>44290</v>
       </c>
@@ -6261,8 +6280,8 @@
       <c r="H58" s="26"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="136"/>
-      <c r="B59" s="140" t="s">
+      <c r="A59" s="140"/>
+      <c r="B59" s="143" t="s">
         <v>86</v>
       </c>
       <c r="C59" s="17">
@@ -6277,8 +6296,8 @@
       <c r="H59" s="21"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="136"/>
-      <c r="B60" s="133"/>
+      <c r="A60" s="140"/>
+      <c r="B60" s="135"/>
       <c r="C60" s="2">
         <v>44292</v>
       </c>
@@ -6293,8 +6312,8 @@
       <c r="H60" s="6"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="136"/>
-      <c r="B61" s="133"/>
+      <c r="A61" s="140"/>
+      <c r="B61" s="135"/>
       <c r="C61" s="2">
         <v>44293</v>
       </c>
@@ -6309,8 +6328,8 @@
       <c r="H61" s="6"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="136"/>
-      <c r="B62" s="133"/>
+      <c r="A62" s="140"/>
+      <c r="B62" s="135"/>
       <c r="C62" s="2">
         <v>44294</v>
       </c>
@@ -6325,8 +6344,8 @@
       <c r="H62" s="6"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="136"/>
-      <c r="B63" s="133"/>
+      <c r="A63" s="140"/>
+      <c r="B63" s="135"/>
       <c r="C63" s="2">
         <v>44295</v>
       </c>
@@ -6337,8 +6356,8 @@
       <c r="H63" s="6"/>
     </row>
     <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="136"/>
-      <c r="B64" s="133"/>
+      <c r="A64" s="140"/>
+      <c r="B64" s="135"/>
       <c r="C64" s="2">
         <v>44296</v>
       </c>
@@ -6349,8 +6368,8 @@
       <c r="H64" s="6"/>
     </row>
     <row r="65" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="136"/>
-      <c r="B65" s="134"/>
+      <c r="A65" s="140"/>
+      <c r="B65" s="136"/>
       <c r="C65" s="22">
         <v>44297</v>
       </c>
@@ -6365,8 +6384,8 @@
       <c r="H65" s="26"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="136"/>
-      <c r="B66" s="132" t="s">
+      <c r="A66" s="140"/>
+      <c r="B66" s="144" t="s">
         <v>82</v>
       </c>
       <c r="C66" s="11">
@@ -6383,8 +6402,8 @@
       <c r="H66" s="15"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="136"/>
-      <c r="B67" s="133"/>
+      <c r="A67" s="140"/>
+      <c r="B67" s="135"/>
       <c r="C67" s="2">
         <v>44299</v>
       </c>
@@ -6399,8 +6418,8 @@
       <c r="H67" s="6"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="136"/>
-      <c r="B68" s="133"/>
+      <c r="A68" s="140"/>
+      <c r="B68" s="135"/>
       <c r="C68" s="2">
         <v>44300</v>
       </c>
@@ -6413,8 +6432,8 @@
       <c r="H68" s="6"/>
     </row>
     <row r="69" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="137"/>
-      <c r="B69" s="134"/>
+      <c r="A69" s="141"/>
+      <c r="B69" s="136"/>
       <c r="C69" s="22">
         <v>44301</v>
       </c>
@@ -6426,11 +6445,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="A51:A69"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="B51:B58"/>
+    <mergeCell ref="B59:B65"/>
     <mergeCell ref="B30:B36"/>
     <mergeCell ref="B21:B29"/>
     <mergeCell ref="B12:B20"/>
@@ -6439,12 +6459,11 @@
     <mergeCell ref="A2:A20"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B37:B43"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="A51:A69"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="B51:B58"/>
-    <mergeCell ref="B59:B65"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6501,10 +6520,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="135" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="135" t="s">
         <v>146</v>
       </c>
       <c r="C2" s="40">
@@ -6523,8 +6542,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="133"/>
-      <c r="B3" s="134"/>
+      <c r="A3" s="135"/>
+      <c r="B3" s="136"/>
       <c r="C3" s="52">
         <v>44094</v>
       </c>
@@ -6541,8 +6560,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="133"/>
-      <c r="B4" s="139" t="s">
+      <c r="A4" s="135"/>
+      <c r="B4" s="137" t="s">
         <v>123</v>
       </c>
       <c r="C4" s="49">
@@ -6561,8 +6580,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="133"/>
-      <c r="B5" s="133"/>
+      <c r="A5" s="135"/>
+      <c r="B5" s="135"/>
       <c r="C5" s="40">
         <v>44096</v>
       </c>
@@ -6579,8 +6598,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="133"/>
-      <c r="B6" s="133"/>
+      <c r="A6" s="135"/>
+      <c r="B6" s="135"/>
       <c r="C6" s="40">
         <v>44097</v>
       </c>
@@ -6597,8 +6616,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="133"/>
-      <c r="B7" s="133"/>
+      <c r="A7" s="135"/>
+      <c r="B7" s="135"/>
       <c r="C7" s="40">
         <v>44098</v>
       </c>
@@ -6615,8 +6634,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="133"/>
-      <c r="B8" s="133"/>
+      <c r="A8" s="135"/>
+      <c r="B8" s="135"/>
       <c r="C8" s="40">
         <v>44099</v>
       </c>
@@ -6633,8 +6652,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="133"/>
-      <c r="B9" s="133"/>
+      <c r="A9" s="135"/>
+      <c r="B9" s="135"/>
       <c r="C9" s="40">
         <v>44100</v>
       </c>
@@ -6651,8 +6670,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="134"/>
-      <c r="B10" s="134"/>
+      <c r="A10" s="136"/>
+      <c r="B10" s="136"/>
       <c r="C10" s="52">
         <v>44101</v>
       </c>
@@ -6669,10 +6688,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="140" t="s">
+      <c r="A11" s="143" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="141" t="s">
+      <c r="B11" s="134" t="s">
         <v>88</v>
       </c>
       <c r="C11" s="57">
@@ -6691,8 +6710,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="133"/>
-      <c r="B12" s="133"/>
+      <c r="A12" s="135"/>
+      <c r="B12" s="135"/>
       <c r="C12" s="40">
         <v>44103</v>
       </c>
@@ -6703,8 +6722,8 @@
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="133"/>
-      <c r="B13" s="133"/>
+      <c r="A13" s="135"/>
+      <c r="B13" s="135"/>
       <c r="C13" s="40">
         <v>44104</v>
       </c>
@@ -6715,8 +6734,8 @@
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="133"/>
-      <c r="B14" s="133"/>
+      <c r="A14" s="135"/>
+      <c r="B14" s="135"/>
       <c r="C14" s="40">
         <v>44105</v>
       </c>
@@ -6731,8 +6750,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="133"/>
-      <c r="B15" s="133"/>
+      <c r="A15" s="135"/>
+      <c r="B15" s="135"/>
       <c r="C15" s="40">
         <v>44106</v>
       </c>
@@ -6749,8 +6768,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="133"/>
-      <c r="B16" s="133"/>
+      <c r="A16" s="135"/>
+      <c r="B16" s="135"/>
       <c r="C16" s="40">
         <v>44107</v>
       </c>
@@ -6767,8 +6786,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="133"/>
-      <c r="B17" s="134"/>
+      <c r="A17" s="135"/>
+      <c r="B17" s="136"/>
       <c r="C17" s="52">
         <v>44108</v>
       </c>
@@ -6785,8 +6804,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="133"/>
-      <c r="B18" s="141" t="s">
+      <c r="A18" s="135"/>
+      <c r="B18" s="134" t="s">
         <v>86</v>
       </c>
       <c r="C18" s="146">
@@ -6805,7 +6824,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="133"/>
+      <c r="A19" s="135"/>
       <c r="B19" s="151"/>
       <c r="C19" s="147"/>
       <c r="D19" s="41" t="s">
@@ -6821,7 +6840,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="133"/>
+      <c r="A20" s="135"/>
       <c r="B20" s="151"/>
       <c r="C20" s="147"/>
       <c r="D20" s="41" t="s">
@@ -6837,8 +6856,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="133"/>
-      <c r="B21" s="133"/>
+      <c r="A21" s="135"/>
+      <c r="B21" s="135"/>
       <c r="C21" s="40">
         <v>44110</v>
       </c>
@@ -6849,8 +6868,8 @@
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="133"/>
-      <c r="B22" s="133"/>
+      <c r="A22" s="135"/>
+      <c r="B22" s="135"/>
       <c r="C22" s="40">
         <v>44111</v>
       </c>
@@ -6861,8 +6880,8 @@
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="133"/>
-      <c r="B23" s="133"/>
+      <c r="A23" s="135"/>
+      <c r="B23" s="135"/>
       <c r="C23" s="40">
         <v>44112</v>
       </c>
@@ -6873,8 +6892,8 @@
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="133"/>
-      <c r="B24" s="133"/>
+      <c r="A24" s="135"/>
+      <c r="B24" s="135"/>
       <c r="C24" s="40">
         <v>44113</v>
       </c>
@@ -6885,8 +6904,8 @@
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="133"/>
-      <c r="B25" s="133"/>
+      <c r="A25" s="135"/>
+      <c r="B25" s="135"/>
       <c r="C25" s="147">
         <v>44114</v>
       </c>
@@ -6903,8 +6922,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="133"/>
-      <c r="B26" s="133"/>
+      <c r="A26" s="135"/>
+      <c r="B26" s="135"/>
       <c r="C26" s="147"/>
       <c r="D26" s="41" t="s">
         <v>102</v>
@@ -6919,8 +6938,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="133"/>
-      <c r="B27" s="134"/>
+      <c r="A27" s="135"/>
+      <c r="B27" s="136"/>
       <c r="C27" s="52">
         <v>44115</v>
       </c>
@@ -6937,8 +6956,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="133"/>
-      <c r="B28" s="141" t="s">
+      <c r="A28" s="135"/>
+      <c r="B28" s="134" t="s">
         <v>82</v>
       </c>
       <c r="C28" s="57">
@@ -6951,8 +6970,8 @@
       <c r="H28" s="21"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="133"/>
-      <c r="B29" s="133"/>
+      <c r="A29" s="135"/>
+      <c r="B29" s="135"/>
       <c r="C29" s="40">
         <v>44117</v>
       </c>
@@ -6969,8 +6988,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="133"/>
-      <c r="B30" s="133"/>
+      <c r="A30" s="135"/>
+      <c r="B30" s="135"/>
       <c r="C30" s="40">
         <v>44118</v>
       </c>
@@ -6981,8 +7000,8 @@
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="133"/>
-      <c r="B31" s="133"/>
+      <c r="A31" s="135"/>
+      <c r="B31" s="135"/>
       <c r="C31" s="40">
         <v>44119</v>
       </c>
@@ -6999,8 +7018,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="133"/>
-      <c r="B32" s="133"/>
+      <c r="A32" s="135"/>
+      <c r="B32" s="135"/>
       <c r="C32" s="40">
         <v>44120</v>
       </c>
@@ -7011,8 +7030,8 @@
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="133"/>
-      <c r="B33" s="133"/>
+      <c r="A33" s="135"/>
+      <c r="B33" s="135"/>
       <c r="C33" s="40">
         <v>44121</v>
       </c>
@@ -7029,8 +7048,8 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="133"/>
-      <c r="B34" s="133"/>
+      <c r="A34" s="135"/>
+      <c r="B34" s="135"/>
       <c r="C34" s="147">
         <v>44122</v>
       </c>
@@ -7047,8 +7066,8 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="133"/>
-      <c r="B35" s="134"/>
+      <c r="A35" s="135"/>
+      <c r="B35" s="136"/>
       <c r="C35" s="148"/>
       <c r="D35" s="53" t="s">
         <v>103</v>
@@ -7063,8 +7082,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="133"/>
-      <c r="B36" s="141" t="s">
+      <c r="A36" s="135"/>
+      <c r="B36" s="134" t="s">
         <v>83</v>
       </c>
       <c r="C36" s="57">
@@ -7077,8 +7096,8 @@
       <c r="H36" s="21"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="133"/>
-      <c r="B37" s="133"/>
+      <c r="A37" s="135"/>
+      <c r="B37" s="135"/>
       <c r="C37" s="40">
         <v>44124</v>
       </c>
@@ -7089,8 +7108,8 @@
       <c r="H37" s="6"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="133"/>
-      <c r="B38" s="133"/>
+      <c r="A38" s="135"/>
+      <c r="B38" s="135"/>
       <c r="C38" s="40">
         <v>44125</v>
       </c>
@@ -7101,8 +7120,8 @@
       <c r="H38" s="6"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="133"/>
-      <c r="B39" s="133"/>
+      <c r="A39" s="135"/>
+      <c r="B39" s="135"/>
       <c r="C39" s="40">
         <v>44126</v>
       </c>
@@ -7113,8 +7132,8 @@
       <c r="H39" s="6"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="133"/>
-      <c r="B40" s="133"/>
+      <c r="A40" s="135"/>
+      <c r="B40" s="135"/>
       <c r="C40" s="40">
         <v>44127</v>
       </c>
@@ -7125,8 +7144,8 @@
       <c r="H40" s="6"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="133"/>
-      <c r="B41" s="133"/>
+      <c r="A41" s="135"/>
+      <c r="B41" s="135"/>
       <c r="C41" s="40">
         <v>44128</v>
       </c>
@@ -7143,8 +7162,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="133"/>
-      <c r="B42" s="134"/>
+      <c r="A42" s="135"/>
+      <c r="B42" s="136"/>
       <c r="C42" s="52">
         <v>44129</v>
       </c>
@@ -7155,8 +7174,8 @@
       <c r="H42" s="26"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="133"/>
-      <c r="B43" s="132" t="s">
+      <c r="A43" s="135"/>
+      <c r="B43" s="144" t="s">
         <v>138</v>
       </c>
       <c r="C43" s="49">
@@ -7175,8 +7194,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="133"/>
-      <c r="B44" s="133"/>
+      <c r="A44" s="135"/>
+      <c r="B44" s="135"/>
       <c r="C44" s="40">
         <v>44131</v>
       </c>
@@ -7193,8 +7212,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="133"/>
-      <c r="B45" s="133"/>
+      <c r="A45" s="135"/>
+      <c r="B45" s="135"/>
       <c r="C45" s="40">
         <v>44132</v>
       </c>
@@ -7211,8 +7230,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="133"/>
-      <c r="B46" s="133"/>
+      <c r="A46" s="135"/>
+      <c r="B46" s="135"/>
       <c r="C46" s="40">
         <v>44133</v>
       </c>
@@ -7223,8 +7242,8 @@
       <c r="H46" s="6"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="133"/>
-      <c r="B47" s="133"/>
+      <c r="A47" s="135"/>
+      <c r="B47" s="135"/>
       <c r="C47" s="40">
         <v>44134</v>
       </c>
@@ -7235,8 +7254,8 @@
       <c r="H47" s="6"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="133"/>
-      <c r="B48" s="133"/>
+      <c r="A48" s="135"/>
+      <c r="B48" s="135"/>
       <c r="C48" s="40">
         <v>44135</v>
       </c>
@@ -7247,8 +7266,8 @@
       <c r="H48" s="6"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="134"/>
-      <c r="B49" s="134"/>
+      <c r="A49" s="136"/>
+      <c r="B49" s="136"/>
       <c r="C49" s="52">
         <v>44136</v>
       </c>
@@ -7265,10 +7284,10 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="140" t="s">
+      <c r="A50" s="143" t="s">
         <v>140</v>
       </c>
-      <c r="B50" s="141" t="s">
+      <c r="B50" s="134" t="s">
         <v>88</v>
       </c>
       <c r="C50" s="57">
@@ -7281,8 +7300,8 @@
       <c r="H50" s="21"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="133"/>
-      <c r="B51" s="133"/>
+      <c r="A51" s="135"/>
+      <c r="B51" s="135"/>
       <c r="C51" s="40">
         <v>44138</v>
       </c>
@@ -7299,8 +7318,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="133"/>
-      <c r="B52" s="133"/>
+      <c r="A52" s="135"/>
+      <c r="B52" s="135"/>
       <c r="C52" s="40">
         <v>44139</v>
       </c>
@@ -7311,8 +7330,8 @@
       <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="133"/>
-      <c r="B53" s="133"/>
+      <c r="A53" s="135"/>
+      <c r="B53" s="135"/>
       <c r="C53" s="40">
         <v>44140</v>
       </c>
@@ -7329,8 +7348,8 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="133"/>
-      <c r="B54" s="133"/>
+      <c r="A54" s="135"/>
+      <c r="B54" s="135"/>
       <c r="C54" s="40">
         <v>44141</v>
       </c>
@@ -7341,8 +7360,8 @@
       <c r="H54" s="6"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="133"/>
-      <c r="B55" s="133"/>
+      <c r="A55" s="135"/>
+      <c r="B55" s="135"/>
       <c r="C55" s="40">
         <v>44142</v>
       </c>
@@ -7353,8 +7372,8 @@
       <c r="H55" s="6"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="133"/>
-      <c r="B56" s="134"/>
+      <c r="A56" s="135"/>
+      <c r="B56" s="136"/>
       <c r="C56" s="52">
         <v>44143</v>
       </c>
@@ -7371,8 +7390,8 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="133"/>
-      <c r="B57" s="141" t="s">
+      <c r="A57" s="135"/>
+      <c r="B57" s="134" t="s">
         <v>86</v>
       </c>
       <c r="C57" s="57">
@@ -7391,8 +7410,8 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="133"/>
-      <c r="B58" s="133"/>
+      <c r="A58" s="135"/>
+      <c r="B58" s="135"/>
       <c r="C58" s="40">
         <v>44145</v>
       </c>
@@ -7409,8 +7428,8 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="133"/>
-      <c r="B59" s="133"/>
+      <c r="A59" s="135"/>
+      <c r="B59" s="135"/>
       <c r="C59" s="40">
         <v>44146</v>
       </c>
@@ -7427,8 +7446,8 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="133"/>
-      <c r="B60" s="133"/>
+      <c r="A60" s="135"/>
+      <c r="B60" s="135"/>
       <c r="C60" s="40">
         <v>44147</v>
       </c>
@@ -7445,8 +7464,8 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="133"/>
-      <c r="B61" s="133"/>
+      <c r="A61" s="135"/>
+      <c r="B61" s="135"/>
       <c r="C61" s="40">
         <v>44148</v>
       </c>
@@ -7457,8 +7476,8 @@
       <c r="H61" s="6"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="133"/>
-      <c r="B62" s="133"/>
+      <c r="A62" s="135"/>
+      <c r="B62" s="135"/>
       <c r="C62" s="40">
         <v>44149</v>
       </c>
@@ -7475,8 +7494,8 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="133"/>
-      <c r="B63" s="134"/>
+      <c r="A63" s="135"/>
+      <c r="B63" s="136"/>
       <c r="C63" s="52">
         <v>44150</v>
       </c>
@@ -7493,8 +7512,8 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="133"/>
-      <c r="B64" s="141" t="s">
+      <c r="A64" s="135"/>
+      <c r="B64" s="134" t="s">
         <v>82</v>
       </c>
       <c r="C64" s="57">
@@ -7513,8 +7532,8 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="133"/>
-      <c r="B65" s="133"/>
+      <c r="A65" s="135"/>
+      <c r="B65" s="135"/>
       <c r="C65" s="40">
         <v>44152</v>
       </c>
@@ -7531,8 +7550,8 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="133"/>
-      <c r="B66" s="133"/>
+      <c r="A66" s="135"/>
+      <c r="B66" s="135"/>
       <c r="C66" s="40">
         <v>44153</v>
       </c>
@@ -7543,8 +7562,8 @@
       <c r="H66" s="6"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="133"/>
-      <c r="B67" s="133"/>
+      <c r="A67" s="135"/>
+      <c r="B67" s="135"/>
       <c r="C67" s="149">
         <v>44154</v>
       </c>
@@ -7561,8 +7580,8 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="133"/>
-      <c r="B68" s="133"/>
+      <c r="A68" s="135"/>
+      <c r="B68" s="135"/>
       <c r="C68" s="150"/>
       <c r="D68" s="41" t="s">
         <v>107</v>
@@ -7577,8 +7596,8 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="133"/>
-      <c r="B69" s="133"/>
+      <c r="A69" s="135"/>
+      <c r="B69" s="135"/>
       <c r="C69" s="40">
         <v>44155</v>
       </c>
@@ -7589,8 +7608,8 @@
       <c r="H69" s="6"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="133"/>
-      <c r="B70" s="133"/>
+      <c r="A70" s="135"/>
+      <c r="B70" s="135"/>
       <c r="C70" s="40">
         <v>44156</v>
       </c>
@@ -7601,8 +7620,8 @@
       <c r="H70" s="6"/>
     </row>
     <row r="71" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="133"/>
-      <c r="B71" s="134"/>
+      <c r="A71" s="135"/>
+      <c r="B71" s="136"/>
       <c r="C71" s="52">
         <v>44157</v>
       </c>
@@ -7619,8 +7638,8 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="133"/>
-      <c r="B72" s="132" t="s">
+      <c r="A72" s="135"/>
+      <c r="B72" s="144" t="s">
         <v>123</v>
       </c>
       <c r="C72" s="49">
@@ -7639,8 +7658,8 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="133"/>
-      <c r="B73" s="133"/>
+      <c r="A73" s="135"/>
+      <c r="B73" s="135"/>
       <c r="C73" s="40">
         <v>44159</v>
       </c>
@@ -7651,8 +7670,8 @@
       <c r="H73" s="6"/>
     </row>
     <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="134"/>
-      <c r="B74" s="134"/>
+      <c r="A74" s="136"/>
+      <c r="B74" s="136"/>
       <c r="C74" s="52">
         <v>44160</v>
       </c>
@@ -7670,6 +7689,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A11:A49"/>
+    <mergeCell ref="A50:A74"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="B11:B17"/>
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="C25:C26"/>
@@ -7681,13 +7707,6 @@
     <mergeCell ref="B18:B27"/>
     <mergeCell ref="B28:B35"/>
     <mergeCell ref="B36:B42"/>
-    <mergeCell ref="A11:A49"/>
-    <mergeCell ref="A50:A74"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="B11:B17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. update scheduler 2. add kafka.emmx
</commit_message>
<xml_diff>
--- a/career/计划&复盘.xlsx
+++ b/career/计划&复盘.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\inotebook\career\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB09F97-B342-492A-9C32-7B95642CDC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F3A40B-3BA9-4D8A-A420-04C5ED91A60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20535" yWindow="3045" windowWidth="16065" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="7月计划" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="238">
   <si>
     <t>JVM</t>
   </si>
@@ -2936,6 +2936,14 @@
   </si>
   <si>
     <t>ZK, Kafka</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:00~25:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12:15~21:15</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3083,7 +3091,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3150,8 +3158,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -3340,11 +3354,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3545,97 +3585,28 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3645,93 +3616,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="58" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3793,7 +3686,199 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="4" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="4" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="4" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="4" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="4" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="4" fillId="12" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="4" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="4" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="4" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4079,8 +4164,8 @@
   <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4093,7 +4178,7 @@
     <col min="6" max="6" width="25" style="39" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.75" style="38" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.75" style="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="113"/>
+    <col min="9" max="9" width="9" style="81"/>
     <col min="10" max="10" width="9" style="37"/>
     <col min="11" max="11" width="7.25" style="37" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.125" style="37" bestFit="1" customWidth="1"/>
@@ -4101,500 +4186,500 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="68" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="68" t="s">
         <v>218</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="H1" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="72" t="s">
+      <c r="I1" s="68" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="103" t="s">
         <v>219</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="74">
+      <c r="B2" s="104"/>
+      <c r="C2" s="105">
         <v>44381</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="69" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="115"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="92"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="130"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="126"/>
-      <c r="B3" s="131" t="s">
+      <c r="A3" s="106"/>
+      <c r="B3" s="107" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="76">
+      <c r="C3" s="108">
         <v>44382</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="116"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="93"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="131"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="126"/>
-      <c r="B4" s="126"/>
-      <c r="C4" s="102">
+      <c r="A4" s="106"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="109">
         <v>44383</v>
       </c>
       <c r="D4" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="117"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="94"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="132"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="126"/>
-      <c r="B5" s="126"/>
-      <c r="C5" s="102">
+      <c r="A5" s="106"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="109">
         <v>44384</v>
       </c>
       <c r="D5" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="117"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="94"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="113"/>
+      <c r="H5" s="113"/>
+      <c r="I5" s="132"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="126"/>
-      <c r="B6" s="126"/>
-      <c r="C6" s="102">
+      <c r="A6" s="106"/>
+      <c r="B6" s="106"/>
+      <c r="C6" s="109">
         <v>44385</v>
       </c>
       <c r="D6" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="117"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="103" t="s">
+      <c r="E6" s="120"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="103">
+      <c r="H6" s="113">
         <v>5</v>
       </c>
-      <c r="I6" s="94"/>
+      <c r="I6" s="132"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="126"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="102">
+      <c r="A7" s="106"/>
+      <c r="B7" s="106"/>
+      <c r="C7" s="109">
         <v>44386</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="113" t="s">
         <v>153</v>
       </c>
-      <c r="E7" s="117"/>
-      <c r="F7" s="88" t="s">
+      <c r="E7" s="120"/>
+      <c r="F7" s="121" t="s">
         <v>150</v>
       </c>
-      <c r="G7" s="103"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="94"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="132"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="126"/>
-      <c r="B8" s="126"/>
-      <c r="C8" s="128">
+      <c r="A8" s="106"/>
+      <c r="B8" s="106"/>
+      <c r="C8" s="110">
         <v>44387</v>
       </c>
-      <c r="D8" s="68" t="s">
+      <c r="D8" s="113" t="s">
         <v>153</v>
       </c>
-      <c r="E8" s="117"/>
-      <c r="F8" s="88" t="s">
+      <c r="E8" s="120"/>
+      <c r="F8" s="121" t="s">
         <v>152</v>
       </c>
-      <c r="G8" s="103" t="s">
+      <c r="G8" s="113" t="s">
         <v>151</v>
       </c>
-      <c r="H8" s="103">
+      <c r="H8" s="113">
         <v>5</v>
       </c>
-      <c r="I8" s="94"/>
+      <c r="I8" s="132"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="126"/>
-      <c r="B9" s="126"/>
-      <c r="C9" s="128"/>
+      <c r="A9" s="106"/>
+      <c r="B9" s="106"/>
+      <c r="C9" s="110"/>
       <c r="D9" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="118">
+      <c r="E9" s="120">
         <v>1.3</v>
       </c>
-      <c r="F9" s="88"/>
-      <c r="G9" s="69" t="s">
+      <c r="F9" s="121"/>
+      <c r="G9" s="122" t="s">
         <v>159</v>
       </c>
-      <c r="H9" s="103">
+      <c r="H9" s="113">
         <v>3</v>
       </c>
-      <c r="I9" s="94"/>
+      <c r="I9" s="132"/>
     </row>
     <row r="10" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="126"/>
-      <c r="B10" s="130"/>
-      <c r="C10" s="79">
+      <c r="A10" s="106"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="112">
         <v>44388</v>
       </c>
-      <c r="D10" s="80" t="s">
+      <c r="D10" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="119" t="s">
+      <c r="E10" s="123" t="s">
         <v>161</v>
       </c>
-      <c r="F10" s="89"/>
-      <c r="G10" s="81" t="s">
+      <c r="F10" s="124"/>
+      <c r="G10" s="125" t="s">
         <v>160</v>
       </c>
-      <c r="H10" s="104">
+      <c r="H10" s="114">
         <v>7</v>
       </c>
-      <c r="I10" s="95"/>
+      <c r="I10" s="133"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="126"/>
-      <c r="B11" s="131" t="s">
+      <c r="A11" s="106"/>
+      <c r="B11" s="107" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="76">
+      <c r="C11" s="108">
         <v>44389</v>
       </c>
-      <c r="D11" s="77" t="s">
+      <c r="D11" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="120">
+      <c r="E11" s="117">
         <v>2.3199999999999998</v>
       </c>
-      <c r="F11" s="82"/>
-      <c r="G11" s="84" t="s">
+      <c r="F11" s="118"/>
+      <c r="G11" s="119" t="s">
         <v>162</v>
       </c>
-      <c r="H11" s="84">
+      <c r="H11" s="119">
         <v>4</v>
       </c>
-      <c r="I11" s="93"/>
-      <c r="L11" s="90" t="s">
+      <c r="I11" s="131"/>
+      <c r="L11" s="72" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="126"/>
-      <c r="B12" s="126"/>
-      <c r="C12" s="102">
+      <c r="A12" s="106"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="109">
         <v>44390</v>
       </c>
       <c r="D12" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="117">
+      <c r="E12" s="120">
         <v>2.4700000000000002</v>
       </c>
-      <c r="F12" s="70"/>
-      <c r="G12" s="103" t="s">
+      <c r="F12" s="121"/>
+      <c r="G12" s="113" t="s">
         <v>162</v>
       </c>
-      <c r="H12" s="103">
+      <c r="H12" s="113">
         <v>4</v>
       </c>
-      <c r="I12" s="94"/>
-      <c r="L12" s="91" t="s">
+      <c r="I12" s="132"/>
+      <c r="L12" s="73" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="126"/>
-      <c r="B13" s="126"/>
-      <c r="C13" s="102">
+      <c r="A13" s="106"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="109">
         <v>44391</v>
       </c>
       <c r="D13" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="121">
+      <c r="E13" s="126">
         <v>2.67</v>
       </c>
-      <c r="F13" s="71"/>
-      <c r="G13" s="103" t="s">
+      <c r="F13" s="127"/>
+      <c r="G13" s="113" t="s">
         <v>162</v>
       </c>
-      <c r="H13" s="103">
+      <c r="H13" s="113">
         <v>4</v>
       </c>
-      <c r="I13" s="94"/>
-      <c r="L13" s="91" t="s">
+      <c r="I13" s="132"/>
+      <c r="L13" s="73" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="126"/>
-      <c r="B14" s="126"/>
-      <c r="C14" s="102">
+      <c r="A14" s="106"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="109">
         <v>44392</v>
       </c>
       <c r="D14" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="117">
+      <c r="E14" s="120">
         <v>2.84</v>
       </c>
-      <c r="F14" s="70"/>
-      <c r="G14" s="103" t="s">
+      <c r="F14" s="121"/>
+      <c r="G14" s="113" t="s">
         <v>163</v>
       </c>
-      <c r="H14" s="103">
+      <c r="H14" s="113">
         <v>4</v>
       </c>
-      <c r="I14" s="94"/>
-      <c r="L14" s="91" t="s">
+      <c r="I14" s="132"/>
+      <c r="L14" s="73" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="126"/>
-      <c r="B15" s="126"/>
-      <c r="C15" s="102">
+      <c r="A15" s="106"/>
+      <c r="B15" s="106"/>
+      <c r="C15" s="109">
         <v>44393</v>
       </c>
-      <c r="D15" s="103"/>
-      <c r="E15" s="117"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="103"/>
-      <c r="H15" s="103"/>
-      <c r="I15" s="94"/>
-      <c r="L15" s="91" t="s">
+      <c r="D15" s="113"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="132"/>
+      <c r="L15" s="73" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="126"/>
-      <c r="B16" s="126"/>
-      <c r="C16" s="102">
+      <c r="A16" s="106"/>
+      <c r="B16" s="106"/>
+      <c r="C16" s="109">
         <v>44394</v>
       </c>
       <c r="D16" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="121" t="s">
+      <c r="E16" s="126" t="s">
         <v>165</v>
       </c>
-      <c r="F16" s="71"/>
-      <c r="G16" s="103" t="s">
+      <c r="F16" s="127"/>
+      <c r="G16" s="113" t="s">
         <v>164</v>
       </c>
-      <c r="H16" s="103">
+      <c r="H16" s="113">
         <v>5</v>
       </c>
-      <c r="I16" s="94"/>
+      <c r="I16" s="132"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="126"/>
-      <c r="B17" s="130"/>
-      <c r="C17" s="79">
+      <c r="A17" s="106"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="112">
         <v>44395</v>
       </c>
-      <c r="D17" s="80" t="s">
+      <c r="D17" s="71" t="s">
         <v>166</v>
       </c>
-      <c r="E17" s="122">
+      <c r="E17" s="123">
         <v>3.41</v>
       </c>
-      <c r="F17" s="83"/>
-      <c r="G17" s="104" t="s">
+      <c r="F17" s="124"/>
+      <c r="G17" s="114" t="s">
         <v>167</v>
       </c>
-      <c r="H17" s="104">
+      <c r="H17" s="114">
         <v>11.5</v>
       </c>
-      <c r="I17" s="95"/>
+      <c r="I17" s="133"/>
     </row>
     <row r="18" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="126"/>
-      <c r="B18" s="131" t="s">
+      <c r="A18" s="106"/>
+      <c r="B18" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="76">
+      <c r="C18" s="108">
         <v>44396</v>
       </c>
-      <c r="D18" s="77" t="s">
+      <c r="D18" s="70" t="s">
         <v>168</v>
       </c>
-      <c r="E18" s="123" t="s">
+      <c r="E18" s="128" t="s">
         <v>170</v>
       </c>
-      <c r="F18" s="85"/>
-      <c r="G18" s="84" t="s">
+      <c r="F18" s="129"/>
+      <c r="G18" s="119" t="s">
         <v>169</v>
       </c>
-      <c r="H18" s="84">
+      <c r="H18" s="119">
         <v>3</v>
       </c>
-      <c r="I18" s="93"/>
-      <c r="L18" s="97" t="s">
+      <c r="I18" s="131"/>
+      <c r="L18" s="75" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="126"/>
-      <c r="B19" s="126"/>
-      <c r="C19" s="102">
+      <c r="A19" s="106"/>
+      <c r="B19" s="106"/>
+      <c r="C19" s="109">
         <v>44397</v>
       </c>
-      <c r="D19" s="68" t="s">
+      <c r="D19" s="113" t="s">
         <v>153</v>
       </c>
-      <c r="E19" s="118" t="s">
+      <c r="E19" s="120" t="s">
         <v>178</v>
       </c>
-      <c r="F19" s="71" t="s">
+      <c r="F19" s="127" t="s">
         <v>171</v>
       </c>
-      <c r="G19" s="103" t="s">
+      <c r="G19" s="113" t="s">
         <v>177</v>
       </c>
-      <c r="H19" s="103">
+      <c r="H19" s="113">
         <v>3</v>
       </c>
-      <c r="I19" s="96" t="s">
+      <c r="I19" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="L19" s="97" t="s">
+      <c r="L19" s="75" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="126"/>
-      <c r="B20" s="126"/>
-      <c r="C20" s="102">
+      <c r="A20" s="106"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="109">
         <v>44398</v>
       </c>
-      <c r="D20" s="68" t="s">
+      <c r="D20" s="113" t="s">
         <v>153</v>
       </c>
-      <c r="E20" s="118" t="s">
+      <c r="E20" s="120" t="s">
         <v>179</v>
       </c>
-      <c r="F20" s="71" t="s">
+      <c r="F20" s="127" t="s">
         <v>171</v>
       </c>
-      <c r="G20" s="103" t="s">
+      <c r="G20" s="113" t="s">
         <v>180</v>
       </c>
-      <c r="H20" s="103">
+      <c r="H20" s="113">
         <v>4</v>
       </c>
-      <c r="I20" s="96" t="s">
+      <c r="I20" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="L20" s="97" t="s">
+      <c r="L20" s="75" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="126"/>
-      <c r="B21" s="126"/>
-      <c r="C21" s="102">
+      <c r="A21" s="106"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="109">
         <v>44399</v>
       </c>
-      <c r="D21" s="68" t="s">
+      <c r="D21" s="113" t="s">
         <v>153</v>
       </c>
-      <c r="E21" s="118" t="s">
+      <c r="E21" s="120" t="s">
         <v>182</v>
       </c>
-      <c r="F21" s="70" t="s">
+      <c r="F21" s="121" t="s">
         <v>172</v>
       </c>
-      <c r="G21" s="103" t="s">
+      <c r="G21" s="113" t="s">
         <v>181</v>
       </c>
-      <c r="H21" s="103">
+      <c r="H21" s="113">
         <v>5</v>
       </c>
-      <c r="I21" s="96" t="s">
+      <c r="I21" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="L21" s="97" t="s">
+      <c r="L21" s="75" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="126"/>
-      <c r="B22" s="126"/>
-      <c r="C22" s="102">
+      <c r="A22" s="106"/>
+      <c r="B22" s="106"/>
+      <c r="C22" s="109">
         <v>44400</v>
       </c>
-      <c r="D22" s="103"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="103"/>
-      <c r="H22" s="103"/>
-      <c r="I22" s="94"/>
-      <c r="L22" s="97" t="s">
+      <c r="D22" s="113"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="121"/>
+      <c r="G22" s="113"/>
+      <c r="H22" s="113"/>
+      <c r="I22" s="132"/>
+      <c r="L22" s="75" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="126"/>
-      <c r="B23" s="126"/>
-      <c r="C23" s="102">
+      <c r="A23" s="106"/>
+      <c r="B23" s="106"/>
+      <c r="C23" s="109">
         <v>44401</v>
       </c>
-      <c r="D23" s="103" t="s">
+      <c r="D23" s="113" t="s">
         <v>153</v>
       </c>
-      <c r="E23" s="118"/>
-      <c r="F23" s="70" t="s">
+      <c r="E23" s="120"/>
+      <c r="F23" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="G23" s="103" t="s">
+      <c r="G23" s="113" t="s">
         <v>189</v>
       </c>
-      <c r="H23" s="103">
+      <c r="H23" s="113">
         <v>7</v>
       </c>
-      <c r="I23" s="96" t="s">
+      <c r="I23" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="L23" s="97" t="s">
+      <c r="L23" s="75" t="s">
         <v>183</v>
       </c>
       <c r="M23" s="39" t="s">
@@ -4603,61 +4688,61 @@
       <c r="N23" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="O23" s="101" t="s">
+      <c r="O23" s="78" t="s">
         <v>208</v>
       </c>
-      <c r="P23" s="101" t="s">
+      <c r="P23" s="78" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="126"/>
-      <c r="B24" s="130"/>
-      <c r="C24" s="79">
+      <c r="A24" s="106"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="112">
         <v>44402</v>
       </c>
-      <c r="D24" s="104" t="s">
+      <c r="D24" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="119"/>
-      <c r="F24" s="83" t="s">
+      <c r="E24" s="123"/>
+      <c r="F24" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="104" t="s">
+      <c r="G24" s="114" t="s">
         <v>201</v>
       </c>
-      <c r="H24" s="104">
+      <c r="H24" s="114">
         <v>5</v>
       </c>
-      <c r="I24" s="95"/>
-      <c r="L24" s="97" t="s">
+      <c r="I24" s="133"/>
+      <c r="L24" s="75" t="s">
         <v>13</v>
       </c>
       <c r="M24" s="38"/>
       <c r="N24" s="38"/>
     </row>
     <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="126"/>
-      <c r="B25" s="131" t="s">
+      <c r="A25" s="106"/>
+      <c r="B25" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="76">
+      <c r="C25" s="108">
         <v>44403</v>
       </c>
-      <c r="D25" s="78" t="s">
+      <c r="D25" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="116"/>
-      <c r="F25" s="82" t="s">
+      <c r="E25" s="117"/>
+      <c r="F25" s="118" t="s">
         <v>187</v>
       </c>
-      <c r="G25" s="105" t="s">
+      <c r="G25" s="134" t="s">
         <v>202</v>
       </c>
-      <c r="H25" s="84">
+      <c r="H25" s="119">
         <v>13</v>
       </c>
-      <c r="I25" s="93"/>
+      <c r="I25" s="131"/>
       <c r="L25" s="38" t="s">
         <v>63</v>
       </c>
@@ -4667,25 +4752,25 @@
       <c r="N25" s="38"/>
     </row>
     <row r="26" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="126"/>
-      <c r="B26" s="126"/>
-      <c r="C26" s="102">
+      <c r="A26" s="106"/>
+      <c r="B26" s="106"/>
+      <c r="C26" s="109">
         <v>44404</v>
       </c>
-      <c r="D26" s="68" t="s">
+      <c r="D26" s="113" t="s">
         <v>204</v>
       </c>
-      <c r="E26" s="118"/>
-      <c r="F26" s="70" t="s">
+      <c r="E26" s="120"/>
+      <c r="F26" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="98" t="s">
+      <c r="G26" s="135" t="s">
         <v>203</v>
       </c>
-      <c r="H26" s="103">
+      <c r="H26" s="113">
         <v>13</v>
       </c>
-      <c r="I26" s="99" t="s">
+      <c r="I26" s="76" t="s">
         <v>4</v>
       </c>
       <c r="L26" s="38" t="s">
@@ -4693,51 +4778,51 @@
       </c>
     </row>
     <row r="27" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="126"/>
-      <c r="B27" s="126"/>
-      <c r="C27" s="102">
+      <c r="A27" s="106"/>
+      <c r="B27" s="106"/>
+      <c r="C27" s="109">
         <v>44405</v>
       </c>
-      <c r="D27" s="68" t="s">
+      <c r="D27" s="113" t="s">
         <v>183</v>
       </c>
-      <c r="E27" s="118"/>
-      <c r="F27" s="70" t="s">
+      <c r="E27" s="120"/>
+      <c r="F27" s="121" t="s">
         <v>175</v>
       </c>
-      <c r="G27" s="98" t="s">
+      <c r="G27" s="135" t="s">
         <v>206</v>
       </c>
-      <c r="H27" s="103">
+      <c r="H27" s="113">
         <v>8</v>
       </c>
-      <c r="I27" s="94"/>
-      <c r="L27" s="38" t="s">
+      <c r="I27" s="132"/>
+      <c r="L27" s="75" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="126"/>
-      <c r="B28" s="126"/>
-      <c r="C28" s="102">
+      <c r="A28" s="106"/>
+      <c r="B28" s="106"/>
+      <c r="C28" s="109">
         <v>44406</v>
       </c>
-      <c r="D28" s="68" t="s">
+      <c r="D28" s="113" t="s">
         <v>183</v>
       </c>
-      <c r="E28" s="118" t="s">
+      <c r="E28" s="120" t="s">
         <v>207</v>
       </c>
-      <c r="F28" s="70" t="s">
+      <c r="F28" s="121" t="s">
         <v>184</v>
       </c>
-      <c r="G28" s="98" t="s">
+      <c r="G28" s="135" t="s">
         <v>209</v>
       </c>
-      <c r="H28" s="103">
+      <c r="H28" s="113">
         <v>11</v>
       </c>
-      <c r="I28" s="100" t="s">
+      <c r="I28" s="77" t="s">
         <v>183</v>
       </c>
       <c r="L28" s="38" t="s">
@@ -4745,79 +4830,79 @@
       </c>
     </row>
     <row r="29" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="126"/>
-      <c r="B29" s="126"/>
-      <c r="C29" s="102">
+      <c r="A29" s="106"/>
+      <c r="B29" s="106"/>
+      <c r="C29" s="109">
         <v>44407</v>
       </c>
-      <c r="D29" s="68" t="s">
+      <c r="D29" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="118" t="s">
+      <c r="E29" s="120" t="s">
         <v>211</v>
       </c>
-      <c r="F29" s="70" t="s">
+      <c r="F29" s="121" t="s">
         <v>186</v>
       </c>
-      <c r="G29" s="98" t="s">
+      <c r="G29" s="135" t="s">
         <v>210</v>
       </c>
-      <c r="H29" s="103">
+      <c r="H29" s="113">
         <v>13</v>
       </c>
-      <c r="I29" s="94"/>
+      <c r="I29" s="132"/>
       <c r="L29" s="38" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="126"/>
-      <c r="B30" s="126"/>
-      <c r="C30" s="102">
+      <c r="A30" s="106"/>
+      <c r="B30" s="106"/>
+      <c r="C30" s="109">
         <v>44408</v>
       </c>
-      <c r="D30" s="68" t="s">
+      <c r="D30" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="118" t="s">
+      <c r="E30" s="120" t="s">
         <v>211</v>
       </c>
-      <c r="F30" s="70" t="s">
+      <c r="F30" s="121" t="s">
         <v>185</v>
       </c>
-      <c r="G30" s="103" t="s">
+      <c r="G30" s="113" t="s">
         <v>212</v>
       </c>
-      <c r="H30" s="103">
+      <c r="H30" s="113">
         <v>9</v>
       </c>
-      <c r="I30" s="94"/>
+      <c r="I30" s="132"/>
       <c r="L30" s="38" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="130"/>
-      <c r="B31" s="130"/>
-      <c r="C31" s="79">
+      <c r="A31" s="111"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="112">
         <v>44409</v>
       </c>
-      <c r="D31" s="104" t="s">
+      <c r="D31" s="114" t="s">
         <v>214</v>
       </c>
-      <c r="E31" s="119" t="s">
+      <c r="E31" s="123" t="s">
         <v>211</v>
       </c>
-      <c r="F31" s="83" t="s">
+      <c r="F31" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="G31" s="104" t="s">
+      <c r="G31" s="114" t="s">
         <v>213</v>
       </c>
-      <c r="H31" s="104">
+      <c r="H31" s="114">
         <v>11</v>
       </c>
-      <c r="I31" s="106" t="s">
+      <c r="I31" s="79" t="s">
         <v>215</v>
       </c>
       <c r="L31" s="38" t="s">
@@ -4825,32 +4910,32 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="127" t="s">
+      <c r="A32" s="166" t="s">
         <v>220</v>
       </c>
-      <c r="B32" s="125" t="s">
+      <c r="B32" s="152" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="108">
+      <c r="C32" s="153">
         <v>44410</v>
       </c>
-      <c r="D32" s="109" t="s">
+      <c r="D32" s="154" t="s">
         <v>216</v>
       </c>
-      <c r="E32" s="124" t="s">
+      <c r="E32" s="155" t="s">
         <v>211</v>
       </c>
-      <c r="F32" s="110" t="s">
+      <c r="F32" s="156" t="s">
         <v>216</v>
       </c>
-      <c r="G32" s="109" t="s">
+      <c r="G32" s="154" t="s">
         <v>224</v>
       </c>
-      <c r="H32" s="109">
+      <c r="H32" s="154">
         <v>3</v>
       </c>
-      <c r="I32" s="111"/>
-      <c r="K32" s="112"/>
+      <c r="I32" s="157"/>
+      <c r="K32" s="80"/>
       <c r="L32" s="38" t="s">
         <v>195</v>
       </c>
@@ -4859,494 +4944,508 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="127"/>
-      <c r="B33" s="126"/>
-      <c r="C33" s="107">
+      <c r="A33" s="136"/>
+      <c r="B33" s="139"/>
+      <c r="C33" s="140">
         <v>44411</v>
       </c>
-      <c r="D33" s="103" t="s">
+      <c r="D33" s="142" t="s">
         <v>216</v>
       </c>
-      <c r="E33" s="117" t="s">
+      <c r="E33" s="145" t="s">
         <v>211</v>
       </c>
-      <c r="F33" s="70" t="s">
+      <c r="F33" s="146" t="s">
         <v>216</v>
       </c>
-      <c r="G33" s="103" t="s">
+      <c r="G33" s="142" t="s">
         <v>225</v>
       </c>
-      <c r="H33" s="103">
+      <c r="H33" s="142">
         <v>4</v>
       </c>
-      <c r="I33" s="94"/>
-      <c r="K33" s="112"/>
+      <c r="I33" s="150"/>
+      <c r="K33" s="80"/>
       <c r="L33" s="38" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="127"/>
-      <c r="B34" s="126"/>
-      <c r="C34" s="107">
+      <c r="A34" s="136"/>
+      <c r="B34" s="139"/>
+      <c r="C34" s="140">
         <v>44412</v>
       </c>
-      <c r="D34" s="103" t="s">
+      <c r="D34" s="142" t="s">
         <v>216</v>
       </c>
-      <c r="E34" s="117" t="s">
+      <c r="E34" s="145" t="s">
         <v>211</v>
       </c>
-      <c r="F34" s="70" t="s">
+      <c r="F34" s="146" t="s">
         <v>175</v>
       </c>
-      <c r="G34" s="69" t="s">
+      <c r="G34" s="147" t="s">
         <v>225</v>
       </c>
-      <c r="H34" s="103">
+      <c r="H34" s="142">
         <v>4</v>
       </c>
-      <c r="I34" s="96" t="s">
+      <c r="I34" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="K34" s="112"/>
+      <c r="K34" s="80"/>
       <c r="L34" s="38" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="127"/>
-      <c r="B35" s="126"/>
-      <c r="C35" s="107">
+      <c r="A35" s="136"/>
+      <c r="B35" s="139"/>
+      <c r="C35" s="140">
         <v>44413</v>
       </c>
-      <c r="D35" s="103" t="s">
+      <c r="D35" s="142" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="117"/>
-      <c r="F35" s="70" t="s">
+      <c r="E35" s="145"/>
+      <c r="F35" s="146" t="s">
         <v>66</v>
       </c>
-      <c r="G35" s="103" t="s">
+      <c r="G35" s="142" t="s">
         <v>226</v>
       </c>
-      <c r="H35" s="103">
+      <c r="H35" s="142">
         <v>2</v>
       </c>
-      <c r="I35" s="94"/>
-      <c r="K35" s="112"/>
+      <c r="I35" s="150"/>
+      <c r="K35" s="80"/>
       <c r="L35" s="38" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="127"/>
-      <c r="B36" s="126"/>
-      <c r="C36" s="107">
+      <c r="A36" s="136"/>
+      <c r="B36" s="139"/>
+      <c r="C36" s="140">
         <v>44414</v>
       </c>
-      <c r="D36" s="103"/>
-      <c r="E36" s="117"/>
-      <c r="F36" s="70" t="s">
+      <c r="D36" s="142"/>
+      <c r="E36" s="145"/>
+      <c r="F36" s="146" t="s">
         <v>70</v>
       </c>
-      <c r="G36" s="103"/>
-      <c r="H36" s="103"/>
-      <c r="I36" s="94"/>
-      <c r="K36" s="112"/>
+      <c r="G36" s="142"/>
+      <c r="H36" s="142"/>
+      <c r="I36" s="150"/>
+      <c r="K36" s="80"/>
       <c r="L36" s="38" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="127"/>
-      <c r="B37" s="126"/>
-      <c r="C37" s="107">
+      <c r="A37" s="136"/>
+      <c r="B37" s="139"/>
+      <c r="C37" s="140">
         <v>44415</v>
       </c>
-      <c r="D37" s="114" t="s">
+      <c r="D37" s="143" t="s">
         <v>228</v>
       </c>
-      <c r="E37" s="117"/>
-      <c r="F37" s="70" t="s">
+      <c r="E37" s="145"/>
+      <c r="F37" s="146" t="s">
         <v>70</v>
       </c>
-      <c r="G37" s="103" t="s">
+      <c r="G37" s="142" t="s">
         <v>227</v>
       </c>
-      <c r="H37" s="103">
+      <c r="H37" s="142">
         <v>11</v>
       </c>
-      <c r="I37" s="94"/>
-      <c r="K37" s="112"/>
+      <c r="I37" s="150"/>
+      <c r="K37" s="80"/>
       <c r="L37" s="38" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="127"/>
-      <c r="B38" s="126"/>
-      <c r="C38" s="107">
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="136"/>
+      <c r="B38" s="158"/>
+      <c r="C38" s="159">
         <v>44416</v>
       </c>
-      <c r="D38" s="152" t="s">
+      <c r="D38" s="160" t="s">
         <v>229</v>
       </c>
-      <c r="E38" s="117" t="s">
+      <c r="E38" s="161" t="s">
         <v>211</v>
       </c>
-      <c r="F38" s="70"/>
-      <c r="G38" s="103" t="s">
+      <c r="F38" s="162"/>
+      <c r="G38" s="163" t="s">
         <v>227</v>
       </c>
-      <c r="H38" s="103">
+      <c r="H38" s="163">
         <v>11</v>
       </c>
-      <c r="I38" s="94"/>
-      <c r="K38" s="112"/>
+      <c r="I38" s="164"/>
+      <c r="K38" s="80"/>
       <c r="L38" s="38" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="127"/>
-      <c r="B39" s="126" t="s">
+      <c r="A39" s="136"/>
+      <c r="B39" s="152" t="s">
         <v>222</v>
       </c>
-      <c r="C39" s="107">
+      <c r="C39" s="153">
         <v>44417</v>
       </c>
-      <c r="D39" s="103" t="s">
+      <c r="D39" s="154" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="117"/>
-      <c r="F39" s="70" t="s">
+      <c r="E39" s="165"/>
+      <c r="F39" s="156" t="s">
         <v>175</v>
       </c>
-      <c r="G39" s="103" t="s">
+      <c r="G39" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="H39" s="103">
+      <c r="H39" s="154">
         <v>3</v>
       </c>
-      <c r="I39" s="94"/>
-      <c r="K39" s="112"/>
+      <c r="I39" s="157"/>
+      <c r="K39" s="80"/>
       <c r="L39" s="38" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="127"/>
-      <c r="B40" s="126"/>
-      <c r="C40" s="107">
+      <c r="A40" s="136"/>
+      <c r="B40" s="139"/>
+      <c r="C40" s="140">
         <v>44418</v>
       </c>
-      <c r="D40" s="103" t="s">
+      <c r="D40" s="142" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="117"/>
-      <c r="F40" s="70" t="s">
+      <c r="E40" s="145"/>
+      <c r="F40" s="146" t="s">
         <v>66</v>
       </c>
-      <c r="G40" s="103" t="s">
+      <c r="G40" s="142" t="s">
         <v>233</v>
       </c>
-      <c r="H40" s="103">
+      <c r="H40" s="142">
         <v>2</v>
       </c>
-      <c r="I40" s="94"/>
-      <c r="K40" s="112"/>
+      <c r="I40" s="150"/>
+      <c r="K40" s="80"/>
       <c r="L40" s="38" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="127"/>
-      <c r="B41" s="126"/>
-      <c r="C41" s="107">
+      <c r="A41" s="136"/>
+      <c r="B41" s="139"/>
+      <c r="C41" s="140">
         <v>44419</v>
       </c>
-      <c r="D41" s="152" t="s">
+      <c r="D41" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="E41" s="117"/>
-      <c r="F41" s="70" t="s">
+      <c r="E41" s="145"/>
+      <c r="F41" s="146" t="s">
         <v>70</v>
       </c>
-      <c r="G41" s="98" t="s">
+      <c r="G41" s="148" t="s">
         <v>234</v>
       </c>
-      <c r="H41" s="103">
+      <c r="H41" s="142">
         <v>3</v>
       </c>
-      <c r="I41" s="94"/>
+      <c r="I41" s="150"/>
       <c r="L41" s="38" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="127"/>
-      <c r="B42" s="126"/>
-      <c r="C42" s="107">
+      <c r="A42" s="136"/>
+      <c r="B42" s="139"/>
+      <c r="C42" s="140">
         <v>44420</v>
       </c>
-      <c r="D42" s="103" t="s">
+      <c r="D42" s="142" t="s">
         <v>235</v>
       </c>
-      <c r="E42" s="117"/>
-      <c r="F42" s="70" t="s">
+      <c r="E42" s="145"/>
+      <c r="F42" s="146" t="s">
         <v>70</v>
       </c>
-      <c r="G42" s="103" t="s">
+      <c r="G42" s="142" t="s">
         <v>232</v>
       </c>
-      <c r="H42" s="103">
+      <c r="H42" s="142">
         <v>3</v>
       </c>
-      <c r="I42" s="94"/>
+      <c r="I42" s="150"/>
       <c r="L42" s="38" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="127"/>
-      <c r="B43" s="126"/>
-      <c r="C43" s="107">
+      <c r="A43" s="136"/>
+      <c r="B43" s="139"/>
+      <c r="C43" s="140">
         <v>44421</v>
       </c>
-      <c r="D43" s="103"/>
-      <c r="E43" s="117"/>
-      <c r="F43" s="70" t="s">
+      <c r="D43" s="142"/>
+      <c r="E43" s="145"/>
+      <c r="F43" s="146" t="s">
         <v>186</v>
       </c>
-      <c r="G43" s="103"/>
-      <c r="H43" s="103"/>
-      <c r="I43" s="94"/>
+      <c r="G43" s="142"/>
+      <c r="H43" s="142"/>
+      <c r="I43" s="150"/>
       <c r="L43" s="38" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="127"/>
-      <c r="B44" s="126"/>
-      <c r="C44" s="107">
+      <c r="A44" s="136"/>
+      <c r="B44" s="139"/>
+      <c r="C44" s="140">
         <v>44422</v>
       </c>
-      <c r="D44" s="103"/>
-      <c r="E44" s="117"/>
-      <c r="F44" s="70" t="s">
+      <c r="D44" s="142" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="145"/>
+      <c r="F44" s="146" t="s">
         <v>230</v>
       </c>
-      <c r="G44" s="103"/>
-      <c r="H44" s="103"/>
-      <c r="I44" s="94"/>
+      <c r="G44" s="142" t="s">
+        <v>236</v>
+      </c>
+      <c r="H44" s="142">
+        <v>9</v>
+      </c>
+      <c r="I44" s="150"/>
       <c r="L44" s="38" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="127"/>
-      <c r="B45" s="126"/>
-      <c r="C45" s="107">
+    <row r="45" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="136"/>
+      <c r="B45" s="158"/>
+      <c r="C45" s="159">
         <v>44423</v>
       </c>
-      <c r="D45" s="103"/>
-      <c r="E45" s="117"/>
-      <c r="F45" s="70" t="s">
+      <c r="D45" s="163" t="s">
+        <v>70</v>
+      </c>
+      <c r="E45" s="161"/>
+      <c r="F45" s="162" t="s">
         <v>231</v>
       </c>
-      <c r="G45" s="103"/>
-      <c r="H45" s="103"/>
-      <c r="I45" s="94"/>
+      <c r="G45" s="163" t="s">
+        <v>237</v>
+      </c>
+      <c r="H45" s="163">
+        <v>9</v>
+      </c>
+      <c r="I45" s="79" t="s">
+        <v>70</v>
+      </c>
       <c r="L45" s="38" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="127"/>
-      <c r="B46" s="126" t="s">
+      <c r="A46" s="136"/>
+      <c r="B46" s="152" t="s">
         <v>223</v>
       </c>
-      <c r="C46" s="107">
+      <c r="C46" s="153">
         <v>44424</v>
       </c>
-      <c r="D46" s="103"/>
-      <c r="E46" s="117"/>
-      <c r="F46" s="70"/>
-      <c r="G46" s="103"/>
-      <c r="H46" s="103"/>
-      <c r="I46" s="94"/>
+      <c r="D46" s="154"/>
+      <c r="E46" s="165"/>
+      <c r="F46" s="156"/>
+      <c r="G46" s="154"/>
+      <c r="H46" s="154"/>
+      <c r="I46" s="157"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="127"/>
-      <c r="B47" s="126"/>
-      <c r="C47" s="107">
+      <c r="A47" s="136"/>
+      <c r="B47" s="139"/>
+      <c r="C47" s="140">
         <v>44425</v>
       </c>
-      <c r="D47" s="103"/>
-      <c r="E47" s="117"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="103"/>
-      <c r="H47" s="103"/>
-      <c r="I47" s="94"/>
+      <c r="D47" s="142"/>
+      <c r="E47" s="145"/>
+      <c r="F47" s="146"/>
+      <c r="G47" s="142"/>
+      <c r="H47" s="142"/>
+      <c r="I47" s="150"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="127"/>
-      <c r="B48" s="126"/>
-      <c r="C48" s="107">
+      <c r="A48" s="136"/>
+      <c r="B48" s="139"/>
+      <c r="C48" s="140">
         <v>44426</v>
       </c>
-      <c r="D48" s="103"/>
-      <c r="E48" s="117"/>
-      <c r="F48" s="70"/>
-      <c r="G48" s="103"/>
-      <c r="H48" s="103"/>
-      <c r="I48" s="94"/>
+      <c r="D48" s="142"/>
+      <c r="E48" s="145"/>
+      <c r="F48" s="146"/>
+      <c r="G48" s="142"/>
+      <c r="H48" s="142"/>
+      <c r="I48" s="150"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="127"/>
-      <c r="B49" s="126"/>
-      <c r="C49" s="107">
+      <c r="A49" s="136"/>
+      <c r="B49" s="139"/>
+      <c r="C49" s="140">
         <v>44427</v>
       </c>
-      <c r="D49" s="103"/>
-      <c r="E49" s="117"/>
-      <c r="F49" s="70"/>
-      <c r="G49" s="103"/>
-      <c r="H49" s="103"/>
-      <c r="I49" s="94"/>
+      <c r="D49" s="142"/>
+      <c r="E49" s="145"/>
+      <c r="F49" s="146"/>
+      <c r="G49" s="142"/>
+      <c r="H49" s="142"/>
+      <c r="I49" s="150"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="127"/>
-      <c r="B50" s="126"/>
-      <c r="C50" s="107">
+      <c r="A50" s="136"/>
+      <c r="B50" s="139"/>
+      <c r="C50" s="140">
         <v>44428</v>
       </c>
-      <c r="D50" s="103"/>
-      <c r="E50" s="117"/>
-      <c r="F50" s="70"/>
-      <c r="G50" s="103"/>
-      <c r="H50" s="103"/>
-      <c r="I50" s="94"/>
+      <c r="D50" s="142"/>
+      <c r="E50" s="145"/>
+      <c r="F50" s="146"/>
+      <c r="G50" s="142"/>
+      <c r="H50" s="142"/>
+      <c r="I50" s="150"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="127"/>
-      <c r="B51" s="126"/>
-      <c r="C51" s="107">
+      <c r="A51" s="136"/>
+      <c r="B51" s="139"/>
+      <c r="C51" s="140">
         <v>44429</v>
       </c>
-      <c r="D51" s="103"/>
-      <c r="E51" s="117"/>
-      <c r="F51" s="70"/>
-      <c r="G51" s="103"/>
-      <c r="H51" s="103"/>
-      <c r="I51" s="94"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="127"/>
-      <c r="B52" s="126"/>
-      <c r="C52" s="107">
+      <c r="D51" s="142"/>
+      <c r="E51" s="145"/>
+      <c r="F51" s="146"/>
+      <c r="G51" s="142"/>
+      <c r="H51" s="142"/>
+      <c r="I51" s="150"/>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="136"/>
+      <c r="B52" s="158"/>
+      <c r="C52" s="159">
         <v>44430</v>
       </c>
-      <c r="D52" s="103"/>
-      <c r="E52" s="117"/>
-      <c r="F52" s="70"/>
-      <c r="G52" s="103"/>
-      <c r="H52" s="103"/>
-      <c r="I52" s="94"/>
+      <c r="D52" s="163"/>
+      <c r="E52" s="161"/>
+      <c r="F52" s="162"/>
+      <c r="G52" s="163"/>
+      <c r="H52" s="163"/>
+      <c r="I52" s="164"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="127"/>
-      <c r="B53" s="126" t="s">
+      <c r="A53" s="136"/>
+      <c r="B53" s="137" t="s">
         <v>123</v>
       </c>
-      <c r="C53" s="107">
+      <c r="C53" s="138">
         <v>44431</v>
       </c>
-      <c r="D53" s="103"/>
-      <c r="E53" s="117"/>
-      <c r="F53" s="70"/>
-      <c r="G53" s="103"/>
-      <c r="H53" s="103"/>
-      <c r="I53" s="94"/>
+      <c r="D53" s="141"/>
+      <c r="E53" s="151"/>
+      <c r="F53" s="144"/>
+      <c r="G53" s="141"/>
+      <c r="H53" s="141"/>
+      <c r="I53" s="149"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="127"/>
-      <c r="B54" s="126"/>
-      <c r="C54" s="107">
+      <c r="A54" s="136"/>
+      <c r="B54" s="139"/>
+      <c r="C54" s="140">
         <v>44432</v>
       </c>
-      <c r="D54" s="103"/>
-      <c r="E54" s="117"/>
-      <c r="F54" s="70"/>
-      <c r="G54" s="103"/>
-      <c r="H54" s="103"/>
-      <c r="I54" s="94"/>
+      <c r="D54" s="142"/>
+      <c r="E54" s="145"/>
+      <c r="F54" s="146"/>
+      <c r="G54" s="142"/>
+      <c r="H54" s="142"/>
+      <c r="I54" s="150"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="127"/>
-      <c r="B55" s="126"/>
-      <c r="C55" s="107">
+      <c r="A55" s="136"/>
+      <c r="B55" s="139"/>
+      <c r="C55" s="140">
         <v>44433</v>
       </c>
-      <c r="D55" s="103"/>
-      <c r="E55" s="117"/>
-      <c r="F55" s="70"/>
-      <c r="G55" s="103"/>
-      <c r="H55" s="103"/>
-      <c r="I55" s="94"/>
+      <c r="D55" s="142"/>
+      <c r="E55" s="145"/>
+      <c r="F55" s="146"/>
+      <c r="G55" s="142"/>
+      <c r="H55" s="142"/>
+      <c r="I55" s="150"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="127"/>
-      <c r="B56" s="126"/>
-      <c r="C56" s="107">
+      <c r="A56" s="136"/>
+      <c r="B56" s="139"/>
+      <c r="C56" s="140">
         <v>44434</v>
       </c>
-      <c r="D56" s="103"/>
-      <c r="E56" s="117"/>
-      <c r="F56" s="70"/>
-      <c r="G56" s="103"/>
-      <c r="H56" s="103"/>
-      <c r="I56" s="94"/>
+      <c r="D56" s="142"/>
+      <c r="E56" s="145"/>
+      <c r="F56" s="146"/>
+      <c r="G56" s="142"/>
+      <c r="H56" s="142"/>
+      <c r="I56" s="150"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="127"/>
-      <c r="B57" s="126"/>
-      <c r="C57" s="107">
+      <c r="A57" s="136"/>
+      <c r="B57" s="139"/>
+      <c r="C57" s="140">
         <v>44435</v>
       </c>
-      <c r="D57" s="103"/>
-      <c r="E57" s="117"/>
-      <c r="F57" s="70"/>
-      <c r="G57" s="103"/>
-      <c r="H57" s="103"/>
-      <c r="I57" s="94"/>
+      <c r="D57" s="142"/>
+      <c r="E57" s="145"/>
+      <c r="F57" s="146"/>
+      <c r="G57" s="142"/>
+      <c r="H57" s="142"/>
+      <c r="I57" s="150"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="127"/>
-      <c r="B58" s="126"/>
-      <c r="C58" s="107">
+      <c r="A58" s="136"/>
+      <c r="B58" s="139"/>
+      <c r="C58" s="140">
         <v>44436</v>
       </c>
-      <c r="D58" s="103"/>
-      <c r="E58" s="117"/>
-      <c r="F58" s="70"/>
-      <c r="G58" s="103"/>
-      <c r="H58" s="103"/>
-      <c r="I58" s="94"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="125"/>
-      <c r="B59" s="126"/>
-      <c r="C59" s="107">
+      <c r="D58" s="142"/>
+      <c r="E58" s="145"/>
+      <c r="F58" s="146"/>
+      <c r="G58" s="142"/>
+      <c r="H58" s="142"/>
+      <c r="I58" s="150"/>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="167"/>
+      <c r="B59" s="158"/>
+      <c r="C59" s="159">
         <v>44437</v>
       </c>
-      <c r="D59" s="103"/>
-      <c r="E59" s="117"/>
-      <c r="F59" s="70"/>
-      <c r="G59" s="103"/>
-      <c r="H59" s="103"/>
-      <c r="I59" s="94"/>
+      <c r="D59" s="163"/>
+      <c r="E59" s="161"/>
+      <c r="F59" s="162"/>
+      <c r="G59" s="163"/>
+      <c r="H59" s="163"/>
+      <c r="I59" s="164"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5418,10 +5517,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="94" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="17">
@@ -5440,8 +5539,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="140"/>
-      <c r="B3" s="136"/>
+      <c r="A3" s="91"/>
+      <c r="B3" s="87"/>
       <c r="C3" s="22">
         <v>44241</v>
       </c>
@@ -5452,8 +5551,8 @@
       <c r="H3" s="26"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="140"/>
-      <c r="B4" s="134" t="s">
+      <c r="A4" s="91"/>
+      <c r="B4" s="85" t="s">
         <v>82</v>
       </c>
       <c r="C4" s="17">
@@ -5472,8 +5571,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="140"/>
-      <c r="B5" s="135"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="86"/>
       <c r="C5" s="2">
         <v>44243</v>
       </c>
@@ -5490,9 +5589,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="140"/>
-      <c r="B6" s="135"/>
-      <c r="C6" s="132">
+      <c r="A6" s="91"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="83">
         <v>44244</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -5508,9 +5607,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="140"/>
-      <c r="B7" s="135"/>
-      <c r="C7" s="133"/>
+      <c r="A7" s="91"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="84"/>
       <c r="D7" s="3" t="s">
         <v>53</v>
       </c>
@@ -5526,8 +5625,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="140"/>
-      <c r="B8" s="135"/>
+      <c r="A8" s="91"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="2">
         <v>44245</v>
       </c>
@@ -5546,8 +5645,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="140"/>
-      <c r="B9" s="135"/>
+      <c r="A9" s="91"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="2">
         <v>44246</v>
       </c>
@@ -5566,8 +5665,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="140"/>
-      <c r="B10" s="135"/>
+      <c r="A10" s="91"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="2">
         <v>44247</v>
       </c>
@@ -5578,8 +5677,8 @@
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="140"/>
-      <c r="B11" s="136"/>
+      <c r="A11" s="91"/>
+      <c r="B11" s="87"/>
       <c r="C11" s="22">
         <v>44248</v>
       </c>
@@ -5596,8 +5695,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="140"/>
-      <c r="B12" s="137" t="s">
+      <c r="A12" s="91"/>
+      <c r="B12" s="88" t="s">
         <v>83</v>
       </c>
       <c r="C12" s="11">
@@ -5612,9 +5711,9 @@
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="140"/>
-      <c r="B13" s="137"/>
-      <c r="C13" s="132">
+      <c r="A13" s="91"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="83">
         <v>44250</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -5628,9 +5727,9 @@
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="140"/>
-      <c r="B14" s="135"/>
-      <c r="C14" s="133"/>
+      <c r="A14" s="91"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="84"/>
       <c r="D14" s="3" t="s">
         <v>60</v>
       </c>
@@ -5642,8 +5741,8 @@
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="140"/>
-      <c r="B15" s="135"/>
+      <c r="A15" s="91"/>
+      <c r="B15" s="86"/>
       <c r="C15" s="2">
         <v>44251</v>
       </c>
@@ -5652,8 +5751,8 @@
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="140"/>
-      <c r="B16" s="135"/>
+      <c r="A16" s="91"/>
+      <c r="B16" s="86"/>
       <c r="C16" s="2">
         <v>44252</v>
       </c>
@@ -5664,8 +5763,8 @@
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="140"/>
-      <c r="B17" s="135"/>
+      <c r="A17" s="91"/>
+      <c r="B17" s="86"/>
       <c r="C17" s="2">
         <v>44253</v>
       </c>
@@ -5676,9 +5775,9 @@
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="140"/>
-      <c r="B18" s="135"/>
-      <c r="C18" s="132">
+      <c r="A18" s="91"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="83">
         <v>44254</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -5690,9 +5789,9 @@
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="142"/>
-      <c r="B19" s="138"/>
-      <c r="C19" s="133"/>
+      <c r="A19" s="93"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="84"/>
       <c r="D19" s="31" t="s">
         <v>62</v>
       </c>
@@ -5702,8 +5801,8 @@
       <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="141"/>
-      <c r="B20" s="136"/>
+      <c r="A20" s="92"/>
+      <c r="B20" s="87"/>
       <c r="C20" s="22">
         <v>44255</v>
       </c>
@@ -5716,10 +5815,10 @@
       <c r="H20" s="26"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="139" t="s">
+      <c r="A21" s="90" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="134" t="s">
+      <c r="B21" s="85" t="s">
         <v>85</v>
       </c>
       <c r="C21" s="17">
@@ -5734,8 +5833,8 @@
       <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="140"/>
-      <c r="B22" s="135"/>
+      <c r="A22" s="91"/>
+      <c r="B22" s="86"/>
       <c r="C22" s="2">
         <v>44257</v>
       </c>
@@ -5748,9 +5847,9 @@
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="140"/>
-      <c r="B23" s="135"/>
-      <c r="C23" s="132">
+      <c r="A23" s="91"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="83">
         <v>44258</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -5762,9 +5861,9 @@
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="140"/>
-      <c r="B24" s="135"/>
-      <c r="C24" s="133"/>
+      <c r="A24" s="91"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="84"/>
       <c r="D24" s="3" t="s">
         <v>66</v>
       </c>
@@ -5776,9 +5875,9 @@
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="140"/>
-      <c r="B25" s="135"/>
-      <c r="C25" s="132">
+      <c r="A25" s="91"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="83">
         <v>44259</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -5792,9 +5891,9 @@
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="140"/>
-      <c r="B26" s="135"/>
-      <c r="C26" s="133"/>
+      <c r="A26" s="91"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="84"/>
       <c r="D26" s="3" t="s">
         <v>69</v>
       </c>
@@ -5804,8 +5903,8 @@
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="140"/>
-      <c r="B27" s="135"/>
+      <c r="A27" s="91"/>
+      <c r="B27" s="86"/>
       <c r="C27" s="2">
         <v>44260</v>
       </c>
@@ -5816,8 +5915,8 @@
       <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="140"/>
-      <c r="B28" s="135"/>
+      <c r="A28" s="91"/>
+      <c r="B28" s="86"/>
       <c r="C28" s="2">
         <v>44261</v>
       </c>
@@ -5828,8 +5927,8 @@
       <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="140"/>
-      <c r="B29" s="136"/>
+      <c r="A29" s="91"/>
+      <c r="B29" s="87"/>
       <c r="C29" s="22">
         <v>44262</v>
       </c>
@@ -5840,8 +5939,8 @@
       <c r="H29" s="26"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="140"/>
-      <c r="B30" s="134" t="s">
+      <c r="A30" s="91"/>
+      <c r="B30" s="85" t="s">
         <v>86</v>
       </c>
       <c r="C30" s="17">
@@ -5854,8 +5953,8 @@
       <c r="H30" s="21"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="140"/>
-      <c r="B31" s="135"/>
+      <c r="A31" s="91"/>
+      <c r="B31" s="86"/>
       <c r="C31" s="2">
         <v>44264</v>
       </c>
@@ -5866,8 +5965,8 @@
       <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="140"/>
-      <c r="B32" s="135"/>
+      <c r="A32" s="91"/>
+      <c r="B32" s="86"/>
       <c r="C32" s="2">
         <v>44265</v>
       </c>
@@ -5878,8 +5977,8 @@
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="140"/>
-      <c r="B33" s="135"/>
+      <c r="A33" s="91"/>
+      <c r="B33" s="86"/>
       <c r="C33" s="2">
         <v>44266</v>
       </c>
@@ -5890,8 +5989,8 @@
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="140"/>
-      <c r="B34" s="135"/>
+      <c r="A34" s="91"/>
+      <c r="B34" s="86"/>
       <c r="C34" s="2">
         <v>44267</v>
       </c>
@@ -5902,8 +6001,8 @@
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="140"/>
-      <c r="B35" s="135"/>
+      <c r="A35" s="91"/>
+      <c r="B35" s="86"/>
       <c r="C35" s="2">
         <v>44268</v>
       </c>
@@ -5914,8 +6013,8 @@
       <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="140"/>
-      <c r="B36" s="136"/>
+      <c r="A36" s="91"/>
+      <c r="B36" s="87"/>
       <c r="C36" s="22">
         <v>44269</v>
       </c>
@@ -5926,8 +6025,8 @@
       <c r="H36" s="26"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="140"/>
-      <c r="B37" s="134" t="s">
+      <c r="A37" s="91"/>
+      <c r="B37" s="85" t="s">
         <v>82</v>
       </c>
       <c r="C37" s="17">
@@ -5942,8 +6041,8 @@
       <c r="H37" s="21"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="140"/>
-      <c r="B38" s="135"/>
+      <c r="A38" s="91"/>
+      <c r="B38" s="86"/>
       <c r="C38" s="2">
         <v>44271</v>
       </c>
@@ -5958,8 +6057,8 @@
       <c r="H38" s="6"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="140"/>
-      <c r="B39" s="135"/>
+      <c r="A39" s="91"/>
+      <c r="B39" s="86"/>
       <c r="C39" s="2">
         <v>44272</v>
       </c>
@@ -5974,8 +6073,8 @@
       <c r="H39" s="6"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="140"/>
-      <c r="B40" s="135"/>
+      <c r="A40" s="91"/>
+      <c r="B40" s="86"/>
       <c r="C40" s="2">
         <v>44273</v>
       </c>
@@ -5990,8 +6089,8 @@
       <c r="H40" s="6"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="140"/>
-      <c r="B41" s="135"/>
+      <c r="A41" s="91"/>
+      <c r="B41" s="86"/>
       <c r="C41" s="2">
         <v>44274</v>
       </c>
@@ -6006,8 +6105,8 @@
       <c r="H41" s="6"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="140"/>
-      <c r="B42" s="135"/>
+      <c r="A42" s="91"/>
+      <c r="B42" s="86"/>
       <c r="C42" s="2">
         <v>44275</v>
       </c>
@@ -6022,8 +6121,8 @@
       <c r="H42" s="6"/>
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="140"/>
-      <c r="B43" s="136"/>
+      <c r="A43" s="91"/>
+      <c r="B43" s="87"/>
       <c r="C43" s="22">
         <v>44276</v>
       </c>
@@ -6038,8 +6137,8 @@
       <c r="H43" s="26"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="140"/>
-      <c r="B44" s="137" t="s">
+      <c r="A44" s="91"/>
+      <c r="B44" s="88" t="s">
         <v>83</v>
       </c>
       <c r="C44" s="11">
@@ -6056,8 +6155,8 @@
       <c r="H44" s="15"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="140"/>
-      <c r="B45" s="135"/>
+      <c r="A45" s="91"/>
+      <c r="B45" s="86"/>
       <c r="C45" s="2">
         <v>44278</v>
       </c>
@@ -6072,8 +6171,8 @@
       <c r="H45" s="6"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="140"/>
-      <c r="B46" s="135"/>
+      <c r="A46" s="91"/>
+      <c r="B46" s="86"/>
       <c r="C46" s="2">
         <v>44279</v>
       </c>
@@ -6090,8 +6189,8 @@
       <c r="H46" s="6"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="140"/>
-      <c r="B47" s="135"/>
+      <c r="A47" s="91"/>
+      <c r="B47" s="86"/>
       <c r="C47" s="2">
         <v>44280</v>
       </c>
@@ -6108,8 +6207,8 @@
       <c r="H47" s="6"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="140"/>
-      <c r="B48" s="135"/>
+      <c r="A48" s="91"/>
+      <c r="B48" s="86"/>
       <c r="C48" s="2">
         <v>44281</v>
       </c>
@@ -6124,8 +6223,8 @@
       <c r="H48" s="6"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="140"/>
-      <c r="B49" s="135"/>
+      <c r="A49" s="91"/>
+      <c r="B49" s="86"/>
       <c r="C49" s="2">
         <v>44282</v>
       </c>
@@ -6142,8 +6241,8 @@
       <c r="H49" s="6"/>
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="141"/>
-      <c r="B50" s="136"/>
+      <c r="A50" s="92"/>
+      <c r="B50" s="87"/>
       <c r="C50" s="22">
         <v>44283</v>
       </c>
@@ -6158,10 +6257,10 @@
       <c r="H50" s="26"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="139" t="s">
+      <c r="A51" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="143" t="s">
+      <c r="B51" s="94" t="s">
         <v>88</v>
       </c>
       <c r="C51" s="17">
@@ -6180,8 +6279,8 @@
       <c r="H51" s="21"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="140"/>
-      <c r="B52" s="135"/>
+      <c r="A52" s="91"/>
+      <c r="B52" s="86"/>
       <c r="C52" s="2">
         <v>44285</v>
       </c>
@@ -6196,9 +6295,9 @@
       <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="140"/>
-      <c r="B53" s="135"/>
-      <c r="C53" s="145">
+      <c r="A53" s="91"/>
+      <c r="B53" s="86"/>
+      <c r="C53" s="96">
         <v>44286</v>
       </c>
       <c r="D53" s="3" t="s">
@@ -6212,9 +6311,9 @@
       <c r="H53" s="6"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="140"/>
-      <c r="B54" s="135"/>
-      <c r="C54" s="145"/>
+      <c r="A54" s="91"/>
+      <c r="B54" s="86"/>
+      <c r="C54" s="96"/>
       <c r="D54" s="3" t="s">
         <v>70</v>
       </c>
@@ -6226,8 +6325,8 @@
       <c r="H54" s="6"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="140"/>
-      <c r="B55" s="135"/>
+      <c r="A55" s="91"/>
+      <c r="B55" s="86"/>
       <c r="C55" s="2">
         <v>44287</v>
       </c>
@@ -6238,8 +6337,8 @@
       <c r="H55" s="6"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="140"/>
-      <c r="B56" s="135"/>
+      <c r="A56" s="91"/>
+      <c r="B56" s="86"/>
       <c r="C56" s="2">
         <v>44288</v>
       </c>
@@ -6252,8 +6351,8 @@
       <c r="H56" s="6"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="140"/>
-      <c r="B57" s="135"/>
+      <c r="A57" s="91"/>
+      <c r="B57" s="86"/>
       <c r="C57" s="2">
         <v>44289</v>
       </c>
@@ -6266,8 +6365,8 @@
       <c r="H57" s="6"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="140"/>
-      <c r="B58" s="136"/>
+      <c r="A58" s="91"/>
+      <c r="B58" s="87"/>
       <c r="C58" s="22">
         <v>44290</v>
       </c>
@@ -6280,8 +6379,8 @@
       <c r="H58" s="26"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="140"/>
-      <c r="B59" s="143" t="s">
+      <c r="A59" s="91"/>
+      <c r="B59" s="94" t="s">
         <v>86</v>
       </c>
       <c r="C59" s="17">
@@ -6296,8 +6395,8 @@
       <c r="H59" s="21"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="140"/>
-      <c r="B60" s="135"/>
+      <c r="A60" s="91"/>
+      <c r="B60" s="86"/>
       <c r="C60" s="2">
         <v>44292</v>
       </c>
@@ -6312,8 +6411,8 @@
       <c r="H60" s="6"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="140"/>
-      <c r="B61" s="135"/>
+      <c r="A61" s="91"/>
+      <c r="B61" s="86"/>
       <c r="C61" s="2">
         <v>44293</v>
       </c>
@@ -6328,8 +6427,8 @@
       <c r="H61" s="6"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="140"/>
-      <c r="B62" s="135"/>
+      <c r="A62" s="91"/>
+      <c r="B62" s="86"/>
       <c r="C62" s="2">
         <v>44294</v>
       </c>
@@ -6344,8 +6443,8 @@
       <c r="H62" s="6"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="140"/>
-      <c r="B63" s="135"/>
+      <c r="A63" s="91"/>
+      <c r="B63" s="86"/>
       <c r="C63" s="2">
         <v>44295</v>
       </c>
@@ -6356,8 +6455,8 @@
       <c r="H63" s="6"/>
     </row>
     <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="140"/>
-      <c r="B64" s="135"/>
+      <c r="A64" s="91"/>
+      <c r="B64" s="86"/>
       <c r="C64" s="2">
         <v>44296</v>
       </c>
@@ -6368,8 +6467,8 @@
       <c r="H64" s="6"/>
     </row>
     <row r="65" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="140"/>
-      <c r="B65" s="136"/>
+      <c r="A65" s="91"/>
+      <c r="B65" s="87"/>
       <c r="C65" s="22">
         <v>44297</v>
       </c>
@@ -6384,8 +6483,8 @@
       <c r="H65" s="26"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="140"/>
-      <c r="B66" s="144" t="s">
+      <c r="A66" s="91"/>
+      <c r="B66" s="95" t="s">
         <v>82</v>
       </c>
       <c r="C66" s="11">
@@ -6402,8 +6501,8 @@
       <c r="H66" s="15"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="140"/>
-      <c r="B67" s="135"/>
+      <c r="A67" s="91"/>
+      <c r="B67" s="86"/>
       <c r="C67" s="2">
         <v>44299</v>
       </c>
@@ -6418,8 +6517,8 @@
       <c r="H67" s="6"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="140"/>
-      <c r="B68" s="135"/>
+      <c r="A68" s="91"/>
+      <c r="B68" s="86"/>
       <c r="C68" s="2">
         <v>44300</v>
       </c>
@@ -6432,8 +6531,8 @@
       <c r="H68" s="6"/>
     </row>
     <row r="69" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="141"/>
-      <c r="B69" s="136"/>
+      <c r="A69" s="92"/>
+      <c r="B69" s="87"/>
       <c r="C69" s="22">
         <v>44301</v>
       </c>
@@ -6520,10 +6619,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="86" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="86" t="s">
         <v>146</v>
       </c>
       <c r="C2" s="40">
@@ -6542,8 +6641,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="135"/>
-      <c r="B3" s="136"/>
+      <c r="A3" s="86"/>
+      <c r="B3" s="87"/>
       <c r="C3" s="52">
         <v>44094</v>
       </c>
@@ -6560,8 +6659,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="135"/>
-      <c r="B4" s="137" t="s">
+      <c r="A4" s="86"/>
+      <c r="B4" s="88" t="s">
         <v>123</v>
       </c>
       <c r="C4" s="49">
@@ -6580,8 +6679,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="135"/>
-      <c r="B5" s="135"/>
+      <c r="A5" s="86"/>
+      <c r="B5" s="86"/>
       <c r="C5" s="40">
         <v>44096</v>
       </c>
@@ -6598,8 +6697,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="135"/>
-      <c r="B6" s="135"/>
+      <c r="A6" s="86"/>
+      <c r="B6" s="86"/>
       <c r="C6" s="40">
         <v>44097</v>
       </c>
@@ -6616,8 +6715,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="135"/>
-      <c r="B7" s="135"/>
+      <c r="A7" s="86"/>
+      <c r="B7" s="86"/>
       <c r="C7" s="40">
         <v>44098</v>
       </c>
@@ -6634,8 +6733,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="135"/>
-      <c r="B8" s="135"/>
+      <c r="A8" s="86"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="40">
         <v>44099</v>
       </c>
@@ -6652,8 +6751,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="135"/>
-      <c r="B9" s="135"/>
+      <c r="A9" s="86"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="40">
         <v>44100</v>
       </c>
@@ -6670,8 +6769,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="136"/>
-      <c r="B10" s="136"/>
+      <c r="A10" s="87"/>
+      <c r="B10" s="87"/>
       <c r="C10" s="52">
         <v>44101</v>
       </c>
@@ -6688,10 +6787,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="143" t="s">
+      <c r="A11" s="94" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="134" t="s">
+      <c r="B11" s="85" t="s">
         <v>88</v>
       </c>
       <c r="C11" s="57">
@@ -6710,8 +6809,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="135"/>
-      <c r="B12" s="135"/>
+      <c r="A12" s="86"/>
+      <c r="B12" s="86"/>
       <c r="C12" s="40">
         <v>44103</v>
       </c>
@@ -6722,8 +6821,8 @@
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="135"/>
-      <c r="B13" s="135"/>
+      <c r="A13" s="86"/>
+      <c r="B13" s="86"/>
       <c r="C13" s="40">
         <v>44104</v>
       </c>
@@ -6734,8 +6833,8 @@
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="135"/>
-      <c r="B14" s="135"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="86"/>
       <c r="C14" s="40">
         <v>44105</v>
       </c>
@@ -6750,8 +6849,8 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="135"/>
-      <c r="B15" s="135"/>
+      <c r="A15" s="86"/>
+      <c r="B15" s="86"/>
       <c r="C15" s="40">
         <v>44106</v>
       </c>
@@ -6768,8 +6867,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="135"/>
-      <c r="B16" s="135"/>
+      <c r="A16" s="86"/>
+      <c r="B16" s="86"/>
       <c r="C16" s="40">
         <v>44107</v>
       </c>
@@ -6786,8 +6885,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="135"/>
-      <c r="B17" s="136"/>
+      <c r="A17" s="86"/>
+      <c r="B17" s="87"/>
       <c r="C17" s="52">
         <v>44108</v>
       </c>
@@ -6804,11 +6903,11 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="135"/>
-      <c r="B18" s="134" t="s">
+      <c r="A18" s="86"/>
+      <c r="B18" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="146">
+      <c r="C18" s="97">
         <v>44109</v>
       </c>
       <c r="D18" s="58" t="s">
@@ -6824,9 +6923,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="135"/>
-      <c r="B19" s="151"/>
-      <c r="C19" s="147"/>
+      <c r="A19" s="86"/>
+      <c r="B19" s="102"/>
+      <c r="C19" s="98"/>
       <c r="D19" s="41" t="s">
         <v>129</v>
       </c>
@@ -6840,9 +6939,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="135"/>
-      <c r="B20" s="151"/>
-      <c r="C20" s="147"/>
+      <c r="A20" s="86"/>
+      <c r="B20" s="102"/>
+      <c r="C20" s="98"/>
       <c r="D20" s="41" t="s">
         <v>101</v>
       </c>
@@ -6856,8 +6955,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="135"/>
-      <c r="B21" s="135"/>
+      <c r="A21" s="86"/>
+      <c r="B21" s="86"/>
       <c r="C21" s="40">
         <v>44110</v>
       </c>
@@ -6868,8 +6967,8 @@
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="135"/>
-      <c r="B22" s="135"/>
+      <c r="A22" s="86"/>
+      <c r="B22" s="86"/>
       <c r="C22" s="40">
         <v>44111</v>
       </c>
@@ -6880,8 +6979,8 @@
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="135"/>
-      <c r="B23" s="135"/>
+      <c r="A23" s="86"/>
+      <c r="B23" s="86"/>
       <c r="C23" s="40">
         <v>44112</v>
       </c>
@@ -6892,8 +6991,8 @@
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="135"/>
-      <c r="B24" s="135"/>
+      <c r="A24" s="86"/>
+      <c r="B24" s="86"/>
       <c r="C24" s="40">
         <v>44113</v>
       </c>
@@ -6904,9 +7003,9 @@
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="135"/>
-      <c r="B25" s="135"/>
-      <c r="C25" s="147">
+      <c r="A25" s="86"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="98">
         <v>44114</v>
       </c>
       <c r="D25" s="41" t="s">
@@ -6922,9 +7021,9 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="135"/>
-      <c r="B26" s="135"/>
-      <c r="C26" s="147"/>
+      <c r="A26" s="86"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="98"/>
       <c r="D26" s="41" t="s">
         <v>102</v>
       </c>
@@ -6938,8 +7037,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="135"/>
-      <c r="B27" s="136"/>
+      <c r="A27" s="86"/>
+      <c r="B27" s="87"/>
       <c r="C27" s="52">
         <v>44115</v>
       </c>
@@ -6956,8 +7055,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="135"/>
-      <c r="B28" s="134" t="s">
+      <c r="A28" s="86"/>
+      <c r="B28" s="85" t="s">
         <v>82</v>
       </c>
       <c r="C28" s="57">
@@ -6970,8 +7069,8 @@
       <c r="H28" s="21"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="135"/>
-      <c r="B29" s="135"/>
+      <c r="A29" s="86"/>
+      <c r="B29" s="86"/>
       <c r="C29" s="40">
         <v>44117</v>
       </c>
@@ -6988,8 +7087,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="135"/>
-      <c r="B30" s="135"/>
+      <c r="A30" s="86"/>
+      <c r="B30" s="86"/>
       <c r="C30" s="40">
         <v>44118</v>
       </c>
@@ -7000,8 +7099,8 @@
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="135"/>
-      <c r="B31" s="135"/>
+      <c r="A31" s="86"/>
+      <c r="B31" s="86"/>
       <c r="C31" s="40">
         <v>44119</v>
       </c>
@@ -7018,8 +7117,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="135"/>
-      <c r="B32" s="135"/>
+      <c r="A32" s="86"/>
+      <c r="B32" s="86"/>
       <c r="C32" s="40">
         <v>44120</v>
       </c>
@@ -7030,8 +7129,8 @@
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="135"/>
-      <c r="B33" s="135"/>
+      <c r="A33" s="86"/>
+      <c r="B33" s="86"/>
       <c r="C33" s="40">
         <v>44121</v>
       </c>
@@ -7048,9 +7147,9 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="135"/>
-      <c r="B34" s="135"/>
-      <c r="C34" s="147">
+      <c r="A34" s="86"/>
+      <c r="B34" s="86"/>
+      <c r="C34" s="98">
         <v>44122</v>
       </c>
       <c r="D34" s="41" t="s">
@@ -7066,9 +7165,9 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="135"/>
-      <c r="B35" s="136"/>
-      <c r="C35" s="148"/>
+      <c r="A35" s="86"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="99"/>
       <c r="D35" s="53" t="s">
         <v>103</v>
       </c>
@@ -7082,8 +7181,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="135"/>
-      <c r="B36" s="134" t="s">
+      <c r="A36" s="86"/>
+      <c r="B36" s="85" t="s">
         <v>83</v>
       </c>
       <c r="C36" s="57">
@@ -7096,8 +7195,8 @@
       <c r="H36" s="21"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="135"/>
-      <c r="B37" s="135"/>
+      <c r="A37" s="86"/>
+      <c r="B37" s="86"/>
       <c r="C37" s="40">
         <v>44124</v>
       </c>
@@ -7108,8 +7207,8 @@
       <c r="H37" s="6"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="135"/>
-      <c r="B38" s="135"/>
+      <c r="A38" s="86"/>
+      <c r="B38" s="86"/>
       <c r="C38" s="40">
         <v>44125</v>
       </c>
@@ -7120,8 +7219,8 @@
       <c r="H38" s="6"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="135"/>
-      <c r="B39" s="135"/>
+      <c r="A39" s="86"/>
+      <c r="B39" s="86"/>
       <c r="C39" s="40">
         <v>44126</v>
       </c>
@@ -7132,8 +7231,8 @@
       <c r="H39" s="6"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="135"/>
-      <c r="B40" s="135"/>
+      <c r="A40" s="86"/>
+      <c r="B40" s="86"/>
       <c r="C40" s="40">
         <v>44127</v>
       </c>
@@ -7144,8 +7243,8 @@
       <c r="H40" s="6"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="135"/>
-      <c r="B41" s="135"/>
+      <c r="A41" s="86"/>
+      <c r="B41" s="86"/>
       <c r="C41" s="40">
         <v>44128</v>
       </c>
@@ -7162,8 +7261,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="135"/>
-      <c r="B42" s="136"/>
+      <c r="A42" s="86"/>
+      <c r="B42" s="87"/>
       <c r="C42" s="52">
         <v>44129</v>
       </c>
@@ -7174,8 +7273,8 @@
       <c r="H42" s="26"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="135"/>
-      <c r="B43" s="144" t="s">
+      <c r="A43" s="86"/>
+      <c r="B43" s="95" t="s">
         <v>138</v>
       </c>
       <c r="C43" s="49">
@@ -7194,8 +7293,8 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="135"/>
-      <c r="B44" s="135"/>
+      <c r="A44" s="86"/>
+      <c r="B44" s="86"/>
       <c r="C44" s="40">
         <v>44131</v>
       </c>
@@ -7212,8 +7311,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="135"/>
-      <c r="B45" s="135"/>
+      <c r="A45" s="86"/>
+      <c r="B45" s="86"/>
       <c r="C45" s="40">
         <v>44132</v>
       </c>
@@ -7230,8 +7329,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="135"/>
-      <c r="B46" s="135"/>
+      <c r="A46" s="86"/>
+      <c r="B46" s="86"/>
       <c r="C46" s="40">
         <v>44133</v>
       </c>
@@ -7242,8 +7341,8 @@
       <c r="H46" s="6"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="135"/>
-      <c r="B47" s="135"/>
+      <c r="A47" s="86"/>
+      <c r="B47" s="86"/>
       <c r="C47" s="40">
         <v>44134</v>
       </c>
@@ -7254,8 +7353,8 @@
       <c r="H47" s="6"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="135"/>
-      <c r="B48" s="135"/>
+      <c r="A48" s="86"/>
+      <c r="B48" s="86"/>
       <c r="C48" s="40">
         <v>44135</v>
       </c>
@@ -7266,8 +7365,8 @@
       <c r="H48" s="6"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="136"/>
-      <c r="B49" s="136"/>
+      <c r="A49" s="87"/>
+      <c r="B49" s="87"/>
       <c r="C49" s="52">
         <v>44136</v>
       </c>
@@ -7284,10 +7383,10 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="143" t="s">
+      <c r="A50" s="94" t="s">
         <v>140</v>
       </c>
-      <c r="B50" s="134" t="s">
+      <c r="B50" s="85" t="s">
         <v>88</v>
       </c>
       <c r="C50" s="57">
@@ -7300,8 +7399,8 @@
       <c r="H50" s="21"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="135"/>
-      <c r="B51" s="135"/>
+      <c r="A51" s="86"/>
+      <c r="B51" s="86"/>
       <c r="C51" s="40">
         <v>44138</v>
       </c>
@@ -7318,8 +7417,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="135"/>
-      <c r="B52" s="135"/>
+      <c r="A52" s="86"/>
+      <c r="B52" s="86"/>
       <c r="C52" s="40">
         <v>44139</v>
       </c>
@@ -7330,8 +7429,8 @@
       <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="135"/>
-      <c r="B53" s="135"/>
+      <c r="A53" s="86"/>
+      <c r="B53" s="86"/>
       <c r="C53" s="40">
         <v>44140</v>
       </c>
@@ -7348,8 +7447,8 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="135"/>
-      <c r="B54" s="135"/>
+      <c r="A54" s="86"/>
+      <c r="B54" s="86"/>
       <c r="C54" s="40">
         <v>44141</v>
       </c>
@@ -7360,8 +7459,8 @@
       <c r="H54" s="6"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="135"/>
-      <c r="B55" s="135"/>
+      <c r="A55" s="86"/>
+      <c r="B55" s="86"/>
       <c r="C55" s="40">
         <v>44142</v>
       </c>
@@ -7372,8 +7471,8 @@
       <c r="H55" s="6"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="135"/>
-      <c r="B56" s="136"/>
+      <c r="A56" s="86"/>
+      <c r="B56" s="87"/>
       <c r="C56" s="52">
         <v>44143</v>
       </c>
@@ -7390,8 +7489,8 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="135"/>
-      <c r="B57" s="134" t="s">
+      <c r="A57" s="86"/>
+      <c r="B57" s="85" t="s">
         <v>86</v>
       </c>
       <c r="C57" s="57">
@@ -7410,8 +7509,8 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="135"/>
-      <c r="B58" s="135"/>
+      <c r="A58" s="86"/>
+      <c r="B58" s="86"/>
       <c r="C58" s="40">
         <v>44145</v>
       </c>
@@ -7428,8 +7527,8 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="135"/>
-      <c r="B59" s="135"/>
+      <c r="A59" s="86"/>
+      <c r="B59" s="86"/>
       <c r="C59" s="40">
         <v>44146</v>
       </c>
@@ -7446,8 +7545,8 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="135"/>
-      <c r="B60" s="135"/>
+      <c r="A60" s="86"/>
+      <c r="B60" s="86"/>
       <c r="C60" s="40">
         <v>44147</v>
       </c>
@@ -7464,8 +7563,8 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="135"/>
-      <c r="B61" s="135"/>
+      <c r="A61" s="86"/>
+      <c r="B61" s="86"/>
       <c r="C61" s="40">
         <v>44148</v>
       </c>
@@ -7476,8 +7575,8 @@
       <c r="H61" s="6"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="135"/>
-      <c r="B62" s="135"/>
+      <c r="A62" s="86"/>
+      <c r="B62" s="86"/>
       <c r="C62" s="40">
         <v>44149</v>
       </c>
@@ -7494,8 +7593,8 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="135"/>
-      <c r="B63" s="136"/>
+      <c r="A63" s="86"/>
+      <c r="B63" s="87"/>
       <c r="C63" s="52">
         <v>44150</v>
       </c>
@@ -7512,8 +7611,8 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="135"/>
-      <c r="B64" s="134" t="s">
+      <c r="A64" s="86"/>
+      <c r="B64" s="85" t="s">
         <v>82</v>
       </c>
       <c r="C64" s="57">
@@ -7532,8 +7631,8 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="135"/>
-      <c r="B65" s="135"/>
+      <c r="A65" s="86"/>
+      <c r="B65" s="86"/>
       <c r="C65" s="40">
         <v>44152</v>
       </c>
@@ -7550,8 +7649,8 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="135"/>
-      <c r="B66" s="135"/>
+      <c r="A66" s="86"/>
+      <c r="B66" s="86"/>
       <c r="C66" s="40">
         <v>44153</v>
       </c>
@@ -7562,9 +7661,9 @@
       <c r="H66" s="6"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="135"/>
-      <c r="B67" s="135"/>
-      <c r="C67" s="149">
+      <c r="A67" s="86"/>
+      <c r="B67" s="86"/>
+      <c r="C67" s="100">
         <v>44154</v>
       </c>
       <c r="D67" s="41" t="s">
@@ -7580,9 +7679,9 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="135"/>
-      <c r="B68" s="135"/>
-      <c r="C68" s="150"/>
+      <c r="A68" s="86"/>
+      <c r="B68" s="86"/>
+      <c r="C68" s="101"/>
       <c r="D68" s="41" t="s">
         <v>107</v>
       </c>
@@ -7596,8 +7695,8 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="135"/>
-      <c r="B69" s="135"/>
+      <c r="A69" s="86"/>
+      <c r="B69" s="86"/>
       <c r="C69" s="40">
         <v>44155</v>
       </c>
@@ -7608,8 +7707,8 @@
       <c r="H69" s="6"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="135"/>
-      <c r="B70" s="135"/>
+      <c r="A70" s="86"/>
+      <c r="B70" s="86"/>
       <c r="C70" s="40">
         <v>44156</v>
       </c>
@@ -7620,8 +7719,8 @@
       <c r="H70" s="6"/>
     </row>
     <row r="71" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="135"/>
-      <c r="B71" s="136"/>
+      <c r="A71" s="86"/>
+      <c r="B71" s="87"/>
       <c r="C71" s="52">
         <v>44157</v>
       </c>
@@ -7638,8 +7737,8 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="135"/>
-      <c r="B72" s="144" t="s">
+      <c r="A72" s="86"/>
+      <c r="B72" s="95" t="s">
         <v>123</v>
       </c>
       <c r="C72" s="49">
@@ -7658,8 +7757,8 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="135"/>
-      <c r="B73" s="135"/>
+      <c r="A73" s="86"/>
+      <c r="B73" s="86"/>
       <c r="C73" s="40">
         <v>44159</v>
       </c>
@@ -7670,8 +7769,8 @@
       <c r="H73" s="6"/>
     </row>
     <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="136"/>
-      <c r="B74" s="136"/>
+      <c r="A74" s="87"/>
+      <c r="B74" s="87"/>
       <c r="C74" s="52">
         <v>44160</v>
       </c>

</xml_diff>